<commit_message>
modified:   Band2MinPowerInput1_FrequencySweepRanges.xlsx 	modified:   config_range5.json
</commit_message>
<xml_diff>
--- a/Band2MinPowerInput1_FrequencySweepRanges.xlsx
+++ b/Band2MinPowerInput1_FrequencySweepRanges.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Test\DVT-Wireless-HCL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hclo365-my.sharepoint.com/personal/aayush_jain_hcl_com/Documents/Facebook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D17B85-349F-4745-B739-B53EBB8D94AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="319" documentId="13_ncr:1_{29D0E568-EE65-415B-89C9-359224AD92FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{E9E78942-3682-4B82-9F5A-C1F40CDDCA2D}"/>
   <bookViews>
-    <workbookView xWindow="2505" yWindow="1335" windowWidth="25500" windowHeight="14265" activeTab="5" xr2:uid="{BA741C37-369C-4D69-BC66-4EE94A3A8637}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{BA741C37-369C-4D69-BC66-4EE94A3A8637}"/>
   </bookViews>
   <sheets>
     <sheet name="Band2" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="91">
   <si>
     <t>Band</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>high</t>
+  </si>
+  <si>
+    <t>Power Level</t>
   </si>
   <si>
     <t>BAND</t>
@@ -328,6 +331,12 @@
   <si>
     <t>UL Frequency</t>
   </si>
+  <si>
+    <t>RB</t>
+  </si>
+  <si>
+    <t>Reduce</t>
+  </si>
 </sst>
 </file>
 
@@ -449,7 +458,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -500,6 +509,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -507,7 +525,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -575,9 +593,10 @@
     <xf numFmtId="165" fontId="4" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="4" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="4" fillId="7" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -895,10 +914,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F21EF5-0615-4121-83E8-517FC8180B1A}">
-  <dimension ref="A1:AH28"/>
+  <dimension ref="A1:AI28"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F13" sqref="F1:F1048576"/>
+    <sheetView topLeftCell="J1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -908,23 +927,23 @@
     <col min="3" max="3" width="18.85546875" style="40" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" style="47" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.140625" style="47" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="69" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" style="40" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" style="38" customWidth="1"/>
     <col min="8" max="10" width="15.7109375" style="38" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.28515625" style="38" customWidth="1"/>
     <col min="12" max="12" width="15.7109375" style="38" bestFit="1" customWidth="1"/>
     <col min="13" max="16" width="15.5703125" style="38" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="19.28515625" style="38" customWidth="1"/>
-    <col min="19" max="19" width="9.140625" style="38"/>
-    <col min="20" max="20" width="24.28515625" style="38" customWidth="1"/>
-    <col min="21" max="21" width="27.5703125" style="38" customWidth="1"/>
-    <col min="22" max="22" width="19.28515625" style="38" customWidth="1"/>
-    <col min="23" max="23" width="12.140625" style="38" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="67.7109375" style="38" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="9.140625" style="38"/>
+    <col min="17" max="19" width="19.28515625" style="38" customWidth="1"/>
+    <col min="20" max="20" width="9.140625" style="38"/>
+    <col min="21" max="21" width="24.28515625" style="38" customWidth="1"/>
+    <col min="22" max="22" width="27.5703125" style="38" customWidth="1"/>
+    <col min="23" max="23" width="19.28515625" style="38" customWidth="1"/>
+    <col min="24" max="24" width="12.140625" style="38" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="67.7109375" style="38" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
@@ -940,53 +959,51 @@
       <c r="E1" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="67" t="s">
+      <c r="F1" s="49" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="37" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="37" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I1" s="37" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J1" s="37" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K1" s="37" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L1" s="37" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="M1" s="37" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="N1" s="37" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="O1" s="37" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="P1" s="37" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="Q1" s="37" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="R1" s="50" t="s">
-        <v>87</v>
-      </c>
-      <c r="T1" s="38" t="s">
-        <v>35</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="S1" s="67"/>
       <c r="U1" s="38" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y1" s="38" t="s">
-        <v>63</v>
+        <v>36</v>
+      </c>
+      <c r="V1" s="38" t="s">
+        <v>46</v>
       </c>
       <c r="Z1" s="38" t="s">
         <v>64</v>
@@ -1015,8 +1032,11 @@
       <c r="AH1" s="38" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AI1" s="38" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="51">
         <v>2</v>
       </c>
@@ -1032,8 +1052,8 @@
       <c r="E2" s="51">
         <v>0</v>
       </c>
-      <c r="F2" s="68">
-        <v>-20</v>
+      <c r="F2" s="52">
+        <v>23</v>
       </c>
       <c r="G2" s="39" t="s">
         <v>7</v>
@@ -1074,23 +1094,21 @@
         <f>C2-80</f>
         <v>1850.7</v>
       </c>
-      <c r="T2" s="38">
-        <v>9000</v>
-      </c>
+      <c r="S2" s="68"/>
       <c r="U2" s="38">
-        <v>30000000</v>
-      </c>
-      <c r="Y2" s="38">
-        <v>1</v>
-      </c>
-      <c r="AA2" s="38" t="s">
-        <v>73</v>
+        <v>9000</v>
+      </c>
+      <c r="V2" s="38">
+        <v>30000000</v>
+      </c>
+      <c r="Z2" s="38">
+        <v>1</v>
       </c>
       <c r="AB2" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AC2" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AD2" s="38" t="s">
         <v>74</v>
@@ -1099,16 +1117,19 @@
         <v>75</v>
       </c>
       <c r="AF2" s="38" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AG2" s="38" t="s">
         <v>76</v>
       </c>
       <c r="AH2" s="38" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="AI2" s="38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" s="51"/>
       <c r="B3" s="39">
         <v>1.4</v>
@@ -1122,8 +1143,8 @@
       <c r="E3" s="51">
         <v>0</v>
       </c>
-      <c r="F3" s="68">
-        <v>-20</v>
+      <c r="F3" s="52">
+        <v>23</v>
       </c>
       <c r="G3" s="39" t="s">
         <v>7</v>
@@ -1164,29 +1185,27 @@
         <f t="shared" ref="R3:R28" si="0">C3-80</f>
         <v>1850.7</v>
       </c>
-      <c r="S3" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="T3" s="38">
-        <v>30000000</v>
-      </c>
-      <c r="U3" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y3" s="38" t="s">
-        <v>73</v>
+      <c r="S3" s="68"/>
+      <c r="T3" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="U3" s="38">
+        <v>30000000</v>
+      </c>
+      <c r="V3" s="38" t="s">
+        <v>49</v>
       </c>
       <c r="Z3" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AA3" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AB3" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AC3" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AD3" s="38" t="s">
         <v>74</v>
@@ -1195,16 +1214,19 @@
         <v>75</v>
       </c>
       <c r="AF3" s="38" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AG3" s="38" t="s">
         <v>76</v>
       </c>
       <c r="AH3" s="38" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="AI3" s="38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="51"/>
       <c r="B4" s="39">
         <v>1.4</v>
@@ -1218,8 +1240,8 @@
       <c r="E4" s="51">
         <v>5</v>
       </c>
-      <c r="F4" s="68">
-        <v>-20</v>
+      <c r="F4" s="52">
+        <v>23</v>
       </c>
       <c r="G4" s="39" t="s">
         <v>7</v>
@@ -1260,32 +1282,30 @@
         <f t="shared" si="0"/>
         <v>1850.7</v>
       </c>
-      <c r="S4" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="T4" s="38">
-        <v>1000000000</v>
-      </c>
-      <c r="U4" s="38" t="s">
-        <v>46</v>
+      <c r="S4" s="68"/>
+      <c r="T4" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="U4" s="38">
+        <v>1000000000</v>
       </c>
       <c r="V4" s="38" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y4" s="38" t="s">
-        <v>73</v>
+        <v>47</v>
+      </c>
+      <c r="W4" s="38" t="s">
+        <v>47</v>
       </c>
       <c r="Z4" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AA4" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AB4" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AC4" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AD4" s="38" t="s">
         <v>74</v>
@@ -1294,16 +1314,19 @@
         <v>75</v>
       </c>
       <c r="AF4" s="38" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AG4" s="38" t="s">
         <v>76</v>
       </c>
       <c r="AH4" s="38" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="AI4" s="38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="51"/>
       <c r="B5" s="39">
         <v>5</v>
@@ -1317,8 +1340,8 @@
       <c r="E5" s="51">
         <v>0</v>
       </c>
-      <c r="F5" s="68">
-        <v>-20</v>
+      <c r="F5" s="52">
+        <v>23</v>
       </c>
       <c r="G5" s="39" t="s">
         <v>7</v>
@@ -1359,32 +1382,30 @@
         <f t="shared" si="0"/>
         <v>1852.5</v>
       </c>
-      <c r="S5" s="38" t="s">
-        <v>44</v>
-      </c>
+      <c r="S5" s="68"/>
       <c r="T5" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="U5" s="38">
-        <v>12750000000</v>
-      </c>
-      <c r="V5" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y5" s="38" t="s">
-        <v>73</v>
+        <v>45</v>
+      </c>
+      <c r="U5" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="V5" s="38">
+        <v>12750000000</v>
+      </c>
+      <c r="W5" s="38" t="s">
+        <v>48</v>
       </c>
       <c r="Z5" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AA5" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AB5" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AC5" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AD5" s="38" t="s">
         <v>74</v>
@@ -1393,16 +1414,19 @@
         <v>75</v>
       </c>
       <c r="AF5" s="38" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AG5" s="38" t="s">
         <v>76</v>
       </c>
       <c r="AH5" s="38" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="AI5" s="38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="51"/>
       <c r="B6" s="39">
         <v>5</v>
@@ -1416,8 +1440,8 @@
       <c r="E6" s="51">
         <v>0</v>
       </c>
-      <c r="F6" s="68">
-        <v>-20</v>
+      <c r="F6" s="52">
+        <v>23</v>
       </c>
       <c r="G6" s="39" t="s">
         <v>7</v>
@@ -1458,20 +1482,18 @@
         <f t="shared" si="0"/>
         <v>1852.5</v>
       </c>
-      <c r="Y6" s="38" t="s">
-        <v>73</v>
-      </c>
+      <c r="S6" s="68"/>
       <c r="Z6" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AA6" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AB6" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AC6" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AD6" s="38" t="s">
         <v>74</v>
@@ -1480,16 +1502,19 @@
         <v>75</v>
       </c>
       <c r="AF6" s="38" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AG6" s="38" t="s">
         <v>76</v>
       </c>
       <c r="AH6" s="38" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="AI6" s="38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="51"/>
       <c r="B7" s="39">
         <v>5</v>
@@ -1503,8 +1528,8 @@
       <c r="E7" s="51">
         <v>24</v>
       </c>
-      <c r="F7" s="68">
-        <v>-20</v>
+      <c r="F7" s="52">
+        <v>23</v>
       </c>
       <c r="G7" s="39" t="s">
         <v>7</v>
@@ -1545,20 +1570,18 @@
         <f t="shared" si="0"/>
         <v>1852.5</v>
       </c>
-      <c r="Y7" s="38" t="s">
-        <v>73</v>
-      </c>
+      <c r="S7" s="68"/>
       <c r="Z7" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AA7" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AB7" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AC7" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AD7" s="38" t="s">
         <v>74</v>
@@ -1567,16 +1590,19 @@
         <v>75</v>
       </c>
       <c r="AF7" s="38" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AG7" s="38" t="s">
         <v>76</v>
       </c>
       <c r="AH7" s="38" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="AI7" s="38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="51"/>
       <c r="B8" s="39">
         <v>20</v>
@@ -1590,8 +1616,8 @@
       <c r="E8" s="51">
         <v>0</v>
       </c>
-      <c r="F8" s="68">
-        <v>-20</v>
+      <c r="F8" s="52">
+        <v>23</v>
       </c>
       <c r="G8" s="39" t="s">
         <v>7</v>
@@ -1632,30 +1658,28 @@
         <f t="shared" si="0"/>
         <v>1860</v>
       </c>
-      <c r="T8" s="38" t="s">
-        <v>49</v>
-      </c>
-      <c r="V8" s="38">
+      <c r="S8" s="68"/>
+      <c r="U8" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="W8" s="38">
         <v>1927200000</v>
       </c>
-      <c r="W8" s="38">
-        <f>V8-W10</f>
+      <c r="X8" s="38">
+        <f>W8-X10</f>
         <v>1927150000</v>
       </c>
-      <c r="Y8" s="38" t="s">
-        <v>73</v>
-      </c>
       <c r="Z8" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AA8" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AB8" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AC8" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AD8" s="38" t="s">
         <v>74</v>
@@ -1664,16 +1688,19 @@
         <v>75</v>
       </c>
       <c r="AF8" s="38" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AG8" s="38" t="s">
         <v>76</v>
       </c>
       <c r="AH8" s="38" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="AI8" s="38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" s="51"/>
       <c r="B9" s="39">
         <v>20</v>
@@ -1687,8 +1714,8 @@
       <c r="E9" s="51">
         <v>0</v>
       </c>
-      <c r="F9" s="68">
-        <v>-20</v>
+      <c r="F9" s="52">
+        <v>23</v>
       </c>
       <c r="G9" s="39" t="s">
         <v>7</v>
@@ -1729,23 +1756,21 @@
         <f t="shared" si="0"/>
         <v>1860</v>
       </c>
-      <c r="T9" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y9" s="38" t="s">
-        <v>73</v>
+      <c r="S9" s="68"/>
+      <c r="U9" s="38" t="s">
+        <v>51</v>
       </c>
       <c r="Z9" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AA9" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AB9" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AC9" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AD9" s="38" t="s">
         <v>74</v>
@@ -1754,16 +1779,19 @@
         <v>75</v>
       </c>
       <c r="AF9" s="38" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AG9" s="38" t="s">
         <v>76</v>
       </c>
       <c r="AH9" s="38" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="AI9" s="38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" s="51"/>
       <c r="B10" s="39">
         <v>20</v>
@@ -1777,8 +1805,8 @@
       <c r="E10" s="51">
         <v>99</v>
       </c>
-      <c r="F10" s="68">
-        <v>-20</v>
+      <c r="F10" s="52">
+        <v>23</v>
       </c>
       <c r="G10" s="39" t="s">
         <v>7</v>
@@ -1819,31 +1847,29 @@
         <f t="shared" si="0"/>
         <v>1860</v>
       </c>
-      <c r="T10" s="40" t="e" cm="1">
-        <f t="array" ref="T10">P</f>
+      <c r="S10" s="68"/>
+      <c r="U10" s="40" t="e" cm="1">
+        <f t="array" ref="U10">P</f>
         <v>#NAME?</v>
       </c>
-      <c r="V10" s="38">
+      <c r="W10" s="38">
         <v>100000</v>
       </c>
-      <c r="W10" s="38">
-        <f>V10/2</f>
+      <c r="X10" s="38">
+        <f>W10/2</f>
         <v>50000</v>
       </c>
-      <c r="Y10" s="38" t="s">
-        <v>73</v>
-      </c>
       <c r="Z10" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AA10" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AB10" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AC10" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AD10" s="38" t="s">
         <v>74</v>
@@ -1852,16 +1878,19 @@
         <v>75</v>
       </c>
       <c r="AF10" s="38" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AG10" s="38" t="s">
         <v>76</v>
       </c>
       <c r="AH10" s="38" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="AI10" s="38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" s="41"/>
       <c r="B11" s="42">
         <v>1.4</v>
@@ -1875,8 +1904,8 @@
       <c r="E11" s="41">
         <v>0</v>
       </c>
-      <c r="F11" s="68">
-        <v>-20</v>
+      <c r="F11" s="43">
+        <v>23</v>
       </c>
       <c r="G11" s="42" t="s">
         <v>8</v>
@@ -1917,20 +1946,18 @@
         <f t="shared" si="0"/>
         <v>1880</v>
       </c>
-      <c r="Y11" s="38" t="s">
-        <v>73</v>
-      </c>
+      <c r="S11" s="68"/>
       <c r="Z11" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AA11" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AB11" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AC11" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AD11" s="38" t="s">
         <v>74</v>
@@ -1939,16 +1966,19 @@
         <v>75</v>
       </c>
       <c r="AF11" s="38" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AG11" s="38" t="s">
         <v>76</v>
       </c>
       <c r="AH11" s="38" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="AI11" s="38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" s="41"/>
       <c r="B12" s="42">
         <v>1.4</v>
@@ -1962,8 +1992,8 @@
       <c r="E12" s="41">
         <v>0</v>
       </c>
-      <c r="F12" s="68">
-        <v>-20</v>
+      <c r="F12" s="43">
+        <v>23</v>
       </c>
       <c r="G12" s="42" t="s">
         <v>8</v>
@@ -2004,20 +2034,18 @@
         <f t="shared" si="0"/>
         <v>1880</v>
       </c>
-      <c r="Y12" s="38" t="s">
-        <v>73</v>
-      </c>
+      <c r="S12" s="68"/>
       <c r="Z12" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AA12" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AB12" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AC12" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AD12" s="38" t="s">
         <v>74</v>
@@ -2026,16 +2054,19 @@
         <v>75</v>
       </c>
       <c r="AF12" s="38" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AG12" s="38" t="s">
         <v>76</v>
       </c>
       <c r="AH12" s="38" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="AI12" s="38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" s="41"/>
       <c r="B13" s="42">
         <v>1.4</v>
@@ -2049,8 +2080,8 @@
       <c r="E13" s="41">
         <v>5</v>
       </c>
-      <c r="F13" s="68">
-        <v>-20</v>
+      <c r="F13" s="43">
+        <v>23</v>
       </c>
       <c r="G13" s="42" t="s">
         <v>8</v>
@@ -2091,20 +2122,18 @@
         <f t="shared" si="0"/>
         <v>1880</v>
       </c>
-      <c r="Y13" s="38" t="s">
-        <v>73</v>
-      </c>
+      <c r="S13" s="68"/>
       <c r="Z13" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AA13" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AB13" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AC13" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AD13" s="38" t="s">
         <v>74</v>
@@ -2113,16 +2142,19 @@
         <v>75</v>
       </c>
       <c r="AF13" s="38" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AG13" s="38" t="s">
         <v>76</v>
       </c>
       <c r="AH13" s="38" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="AI13" s="38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" s="41"/>
       <c r="B14" s="42">
         <v>5</v>
@@ -2136,8 +2168,8 @@
       <c r="E14" s="41">
         <v>0</v>
       </c>
-      <c r="F14" s="68">
-        <v>-20</v>
+      <c r="F14" s="43">
+        <v>23</v>
       </c>
       <c r="G14" s="42" t="s">
         <v>8</v>
@@ -2178,20 +2210,18 @@
         <f t="shared" si="0"/>
         <v>1880</v>
       </c>
-      <c r="Y14" s="38" t="s">
-        <v>73</v>
-      </c>
+      <c r="S14" s="68"/>
       <c r="Z14" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AA14" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AB14" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AC14" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AD14" s="38" t="s">
         <v>74</v>
@@ -2200,16 +2230,19 @@
         <v>75</v>
       </c>
       <c r="AF14" s="38" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AG14" s="38" t="s">
         <v>76</v>
       </c>
       <c r="AH14" s="38" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="AI14" s="38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" s="41"/>
       <c r="B15" s="42">
         <v>5</v>
@@ -2223,8 +2256,8 @@
       <c r="E15" s="41">
         <v>0</v>
       </c>
-      <c r="F15" s="68">
-        <v>-20</v>
+      <c r="F15" s="43">
+        <v>23</v>
       </c>
       <c r="G15" s="42" t="s">
         <v>8</v>
@@ -2265,23 +2298,21 @@
         <f t="shared" si="0"/>
         <v>1880</v>
       </c>
-      <c r="V15" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y15" s="38" t="s">
-        <v>73</v>
+      <c r="S15" s="68"/>
+      <c r="W15" s="38" t="s">
+        <v>52</v>
       </c>
       <c r="Z15" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AA15" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AB15" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AC15" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AD15" s="38" t="s">
         <v>74</v>
@@ -2290,16 +2321,19 @@
         <v>75</v>
       </c>
       <c r="AF15" s="38" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AG15" s="38" t="s">
         <v>76</v>
       </c>
       <c r="AH15" s="38" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="AI15" s="38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" s="41"/>
       <c r="B16" s="42">
         <v>5</v>
@@ -2313,8 +2347,8 @@
       <c r="E16" s="41">
         <v>24</v>
       </c>
-      <c r="F16" s="68">
-        <v>-20</v>
+      <c r="F16" s="43">
+        <v>23</v>
       </c>
       <c r="G16" s="42" t="s">
         <v>8</v>
@@ -2355,23 +2389,21 @@
         <f t="shared" si="0"/>
         <v>1880</v>
       </c>
-      <c r="X16" s="38" t="s">
-        <v>52</v>
-      </c>
+      <c r="S16" s="68"/>
       <c r="Y16" s="38" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="Z16" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AA16" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AB16" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AC16" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AD16" s="38" t="s">
         <v>74</v>
@@ -2380,16 +2412,19 @@
         <v>75</v>
       </c>
       <c r="AF16" s="38" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AG16" s="38" t="s">
         <v>76</v>
       </c>
       <c r="AH16" s="38" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="AI16" s="38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" s="41"/>
       <c r="B17" s="42">
         <v>20</v>
@@ -2403,8 +2438,8 @@
       <c r="E17" s="41">
         <v>0</v>
       </c>
-      <c r="F17" s="68">
-        <v>-20</v>
+      <c r="F17" s="43">
+        <v>23</v>
       </c>
       <c r="G17" s="42" t="s">
         <v>8</v>
@@ -2445,23 +2480,21 @@
         <f t="shared" si="0"/>
         <v>1880</v>
       </c>
-      <c r="X17" s="38" t="s">
-        <v>53</v>
-      </c>
+      <c r="S17" s="68"/>
       <c r="Y17" s="38" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="Z17" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AA17" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AB17" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AC17" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AD17" s="38" t="s">
         <v>74</v>
@@ -2470,16 +2503,19 @@
         <v>75</v>
       </c>
       <c r="AF17" s="38" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AG17" s="38" t="s">
         <v>76</v>
       </c>
       <c r="AH17" s="38" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="AI17" s="38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18" s="41"/>
       <c r="B18" s="42">
         <v>20</v>
@@ -2493,8 +2529,8 @@
       <c r="E18" s="41">
         <v>0</v>
       </c>
-      <c r="F18" s="68">
-        <v>-20</v>
+      <c r="F18" s="43">
+        <v>23</v>
       </c>
       <c r="G18" s="42" t="s">
         <v>8</v>
@@ -2535,23 +2571,21 @@
         <f t="shared" si="0"/>
         <v>1880</v>
       </c>
-      <c r="X18" s="38" t="s">
-        <v>54</v>
-      </c>
+      <c r="S18" s="68"/>
       <c r="Y18" s="38" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="Z18" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AA18" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AB18" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AC18" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AD18" s="38" t="s">
         <v>74</v>
@@ -2560,16 +2594,19 @@
         <v>75</v>
       </c>
       <c r="AF18" s="38" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AG18" s="38" t="s">
         <v>76</v>
       </c>
       <c r="AH18" s="38" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="AI18" s="38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19" s="41"/>
       <c r="B19" s="42">
         <v>20</v>
@@ -2583,8 +2620,8 @@
       <c r="E19" s="41">
         <v>99</v>
       </c>
-      <c r="F19" s="68">
-        <v>-20</v>
+      <c r="F19" s="43">
+        <v>23</v>
       </c>
       <c r="G19" s="42" t="s">
         <v>8</v>
@@ -2625,23 +2662,21 @@
         <f t="shared" si="0"/>
         <v>1880</v>
       </c>
-      <c r="X19" s="38" t="s">
-        <v>55</v>
-      </c>
+      <c r="S19" s="68"/>
       <c r="Y19" s="38" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="Z19" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AA19" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AB19" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AC19" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AD19" s="38" t="s">
         <v>74</v>
@@ -2650,16 +2685,19 @@
         <v>75</v>
       </c>
       <c r="AF19" s="38" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AG19" s="38" t="s">
         <v>76</v>
       </c>
       <c r="AH19" s="38" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="AI19" s="38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20" s="44"/>
       <c r="B20" s="45">
         <v>1.4</v>
@@ -2673,8 +2711,8 @@
       <c r="E20" s="44">
         <v>0</v>
       </c>
-      <c r="F20" s="68">
-        <v>-20</v>
+      <c r="F20" s="46">
+        <v>23</v>
       </c>
       <c r="G20" s="45" t="s">
         <v>9</v>
@@ -2715,23 +2753,21 @@
         <f t="shared" si="0"/>
         <v>1909.3</v>
       </c>
-      <c r="V20" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y20" s="38" t="s">
-        <v>73</v>
+      <c r="S20" s="68"/>
+      <c r="W20" s="38" t="s">
+        <v>57</v>
       </c>
       <c r="Z20" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AA20" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AB20" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AC20" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AD20" s="38" t="s">
         <v>74</v>
@@ -2740,16 +2776,19 @@
         <v>75</v>
       </c>
       <c r="AF20" s="38" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AG20" s="38" t="s">
         <v>76</v>
       </c>
       <c r="AH20" s="38" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="AI20" s="38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21" s="44"/>
       <c r="B21" s="45">
         <v>1.4</v>
@@ -2763,8 +2802,8 @@
       <c r="E21" s="44">
         <v>0</v>
       </c>
-      <c r="F21" s="68">
-        <v>-20</v>
+      <c r="F21" s="46">
+        <v>23</v>
       </c>
       <c r="G21" s="45" t="s">
         <v>9</v>
@@ -2805,23 +2844,21 @@
         <f t="shared" si="0"/>
         <v>1909.3</v>
       </c>
-      <c r="X21" s="38" t="s">
-        <v>57</v>
-      </c>
+      <c r="S21" s="68"/>
       <c r="Y21" s="38" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="Z21" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AA21" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AB21" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AC21" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AD21" s="38" t="s">
         <v>74</v>
@@ -2830,16 +2867,19 @@
         <v>75</v>
       </c>
       <c r="AF21" s="38" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AG21" s="38" t="s">
         <v>76</v>
       </c>
       <c r="AH21" s="38" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="AI21" s="38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22" s="44"/>
       <c r="B22" s="45">
         <v>1.4</v>
@@ -2853,8 +2893,8 @@
       <c r="E22" s="44">
         <v>5</v>
       </c>
-      <c r="F22" s="68">
-        <v>-20</v>
+      <c r="F22" s="46">
+        <v>23</v>
       </c>
       <c r="G22" s="45" t="s">
         <v>9</v>
@@ -2895,23 +2935,21 @@
         <f t="shared" si="0"/>
         <v>1909.3</v>
       </c>
-      <c r="X22" s="38" t="s">
-        <v>58</v>
-      </c>
+      <c r="S22" s="68"/>
       <c r="Y22" s="38" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="Z22" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AA22" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AB22" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AC22" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AD22" s="38" t="s">
         <v>74</v>
@@ -2920,16 +2958,19 @@
         <v>75</v>
       </c>
       <c r="AF22" s="38" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AG22" s="38" t="s">
         <v>76</v>
       </c>
       <c r="AH22" s="38" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="AI22" s="38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23" s="44"/>
       <c r="B23" s="45">
         <v>5</v>
@@ -2943,8 +2984,8 @@
       <c r="E23" s="44">
         <v>0</v>
       </c>
-      <c r="F23" s="68">
-        <v>-20</v>
+      <c r="F23" s="46">
+        <v>23</v>
       </c>
       <c r="G23" s="45" t="s">
         <v>9</v>
@@ -2985,23 +3026,21 @@
         <f t="shared" si="0"/>
         <v>1907.5</v>
       </c>
-      <c r="X23" s="38" t="s">
-        <v>59</v>
-      </c>
+      <c r="S23" s="68"/>
       <c r="Y23" s="38" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="Z23" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AA23" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AB23" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AC23" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AD23" s="38" t="s">
         <v>74</v>
@@ -3010,16 +3049,19 @@
         <v>75</v>
       </c>
       <c r="AF23" s="38" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AG23" s="38" t="s">
         <v>76</v>
       </c>
       <c r="AH23" s="38" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="AI23" s="38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24" s="44"/>
       <c r="B24" s="45">
         <v>5</v>
@@ -3033,8 +3075,8 @@
       <c r="E24" s="44">
         <v>0</v>
       </c>
-      <c r="F24" s="68">
-        <v>-20</v>
+      <c r="F24" s="46">
+        <v>23</v>
       </c>
       <c r="G24" s="45" t="s">
         <v>9</v>
@@ -3075,23 +3117,21 @@
         <f t="shared" si="0"/>
         <v>1907.5</v>
       </c>
-      <c r="X24" s="38" t="s">
-        <v>60</v>
-      </c>
+      <c r="S24" s="68"/>
       <c r="Y24" s="38" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Z24" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AA24" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AB24" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AC24" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AD24" s="38" t="s">
         <v>74</v>
@@ -3100,16 +3140,19 @@
         <v>75</v>
       </c>
       <c r="AF24" s="38" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AG24" s="38" t="s">
         <v>76</v>
       </c>
       <c r="AH24" s="38" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="AI24" s="38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25" s="44"/>
       <c r="B25" s="45">
         <v>5</v>
@@ -3123,8 +3166,8 @@
       <c r="E25" s="44">
         <v>24</v>
       </c>
-      <c r="F25" s="68">
-        <v>-20</v>
+      <c r="F25" s="46">
+        <v>23</v>
       </c>
       <c r="G25" s="45" t="s">
         <v>9</v>
@@ -3165,20 +3208,18 @@
         <f t="shared" si="0"/>
         <v>1907.5</v>
       </c>
-      <c r="Y25" s="38" t="s">
-        <v>73</v>
-      </c>
+      <c r="S25" s="68"/>
       <c r="Z25" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AA25" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AB25" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AC25" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AD25" s="38" t="s">
         <v>74</v>
@@ -3187,16 +3228,19 @@
         <v>75</v>
       </c>
       <c r="AF25" s="38" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AG25" s="38" t="s">
         <v>76</v>
       </c>
       <c r="AH25" s="38" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="AI25" s="38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26" s="44"/>
       <c r="B26" s="45">
         <v>20</v>
@@ -3210,8 +3254,8 @@
       <c r="E26" s="44">
         <v>0</v>
       </c>
-      <c r="F26" s="68">
-        <v>-20</v>
+      <c r="F26" s="46">
+        <v>23</v>
       </c>
       <c r="G26" s="45" t="s">
         <v>9</v>
@@ -3252,23 +3296,21 @@
         <f t="shared" si="0"/>
         <v>1900</v>
       </c>
-      <c r="X26" s="38" t="s">
-        <v>61</v>
-      </c>
+      <c r="S26" s="68"/>
       <c r="Y26" s="38" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="Z26" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AA26" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AB26" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AC26" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AD26" s="38" t="s">
         <v>74</v>
@@ -3277,16 +3319,19 @@
         <v>75</v>
       </c>
       <c r="AF26" s="38" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AG26" s="38" t="s">
         <v>76</v>
       </c>
       <c r="AH26" s="38" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="AI26" s="38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27" s="44"/>
       <c r="B27" s="45">
         <v>20</v>
@@ -3300,8 +3345,8 @@
       <c r="E27" s="44">
         <v>0</v>
       </c>
-      <c r="F27" s="68">
-        <v>-20</v>
+      <c r="F27" s="46">
+        <v>23</v>
       </c>
       <c r="G27" s="45" t="s">
         <v>9</v>
@@ -3342,23 +3387,21 @@
         <f t="shared" si="0"/>
         <v>1900</v>
       </c>
-      <c r="X27" s="38" t="s">
-        <v>62</v>
-      </c>
+      <c r="S27" s="68"/>
       <c r="Y27" s="38" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="Z27" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AA27" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AB27" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AC27" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AD27" s="38" t="s">
         <v>74</v>
@@ -3367,16 +3410,19 @@
         <v>75</v>
       </c>
       <c r="AF27" s="38" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AG27" s="38" t="s">
         <v>76</v>
       </c>
       <c r="AH27" s="38" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="AI27" s="38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A28" s="44"/>
       <c r="B28" s="45">
         <v>20</v>
@@ -3390,8 +3436,8 @@
       <c r="E28" s="44">
         <v>99</v>
       </c>
-      <c r="F28" s="68">
-        <v>-20</v>
+      <c r="F28" s="46">
+        <v>23</v>
       </c>
       <c r="G28" s="45" t="s">
         <v>9</v>
@@ -3432,20 +3478,18 @@
         <f t="shared" si="0"/>
         <v>1900</v>
       </c>
-      <c r="Y28" s="38" t="s">
-        <v>73</v>
-      </c>
+      <c r="S28" s="68"/>
       <c r="Z28" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AA28" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AB28" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AC28" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AD28" s="38" t="s">
         <v>74</v>
@@ -3454,13 +3498,16 @@
         <v>75</v>
       </c>
       <c r="AF28" s="38" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AG28" s="38" t="s">
         <v>76</v>
       </c>
       <c r="AH28" s="38" t="s">
-        <v>73</v>
+        <v>77</v>
+      </c>
+      <c r="AI28" s="38" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -3478,7 +3525,7 @@
   <dimension ref="A1:R28"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3487,7 +3534,7 @@
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="69" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
     <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="16.85546875" customWidth="1"/>
     <col min="10" max="10" width="15.5703125" customWidth="1"/>
@@ -3517,44 +3564,44 @@
       <c r="E1" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="67" t="s">
+      <c r="F1" s="49" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="37" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="37" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I1" s="37" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J1" s="37" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K1" s="37" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L1" s="37" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="M1" s="37" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="N1" s="37" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="O1" s="37" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="P1" s="37" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="Q1" s="37" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="R1" s="50" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -3573,8 +3620,8 @@
       <c r="E2" s="51">
         <v>0</v>
       </c>
-      <c r="F2" s="68">
-        <v>-20</v>
+      <c r="F2" s="52">
+        <v>23</v>
       </c>
       <c r="G2" s="39" t="s">
         <v>7</v>
@@ -3630,8 +3677,8 @@
       <c r="E3" s="51">
         <v>0</v>
       </c>
-      <c r="F3" s="68">
-        <v>-20</v>
+      <c r="F3" s="52">
+        <v>23</v>
       </c>
       <c r="G3" s="39" t="s">
         <v>7</v>
@@ -3687,8 +3734,8 @@
       <c r="E4" s="51">
         <v>5</v>
       </c>
-      <c r="F4" s="68">
-        <v>-20</v>
+      <c r="F4" s="52">
+        <v>23</v>
       </c>
       <c r="G4" s="39" t="s">
         <v>7</v>
@@ -3744,8 +3791,8 @@
       <c r="E5" s="51">
         <v>0</v>
       </c>
-      <c r="F5" s="68">
-        <v>-20</v>
+      <c r="F5" s="52">
+        <v>23</v>
       </c>
       <c r="G5" s="39" t="s">
         <v>7</v>
@@ -3801,8 +3848,8 @@
       <c r="E6" s="51">
         <v>0</v>
       </c>
-      <c r="F6" s="68">
-        <v>-20</v>
+      <c r="F6" s="52">
+        <v>23</v>
       </c>
       <c r="G6" s="39" t="s">
         <v>7</v>
@@ -3858,8 +3905,8 @@
       <c r="E7" s="51">
         <v>24</v>
       </c>
-      <c r="F7" s="68">
-        <v>-20</v>
+      <c r="F7" s="52">
+        <v>23</v>
       </c>
       <c r="G7" s="39" t="s">
         <v>7</v>
@@ -3915,8 +3962,8 @@
       <c r="E8" s="51">
         <v>0</v>
       </c>
-      <c r="F8" s="68">
-        <v>-20</v>
+      <c r="F8" s="52">
+        <v>23</v>
       </c>
       <c r="G8" s="39" t="s">
         <v>7</v>
@@ -3972,8 +4019,8 @@
       <c r="E9" s="51">
         <v>0</v>
       </c>
-      <c r="F9" s="68">
-        <v>-20</v>
+      <c r="F9" s="52">
+        <v>23</v>
       </c>
       <c r="G9" s="39" t="s">
         <v>7</v>
@@ -4029,8 +4076,8 @@
       <c r="E10" s="51">
         <v>99</v>
       </c>
-      <c r="F10" s="68">
-        <v>-20</v>
+      <c r="F10" s="52">
+        <v>23</v>
       </c>
       <c r="G10" s="39" t="s">
         <v>7</v>
@@ -4086,8 +4133,8 @@
       <c r="E11" s="41">
         <v>0</v>
       </c>
-      <c r="F11" s="68">
-        <v>-20</v>
+      <c r="F11" s="43">
+        <v>23</v>
       </c>
       <c r="G11" s="42" t="s">
         <v>8</v>
@@ -4143,8 +4190,8 @@
       <c r="E12" s="41">
         <v>0</v>
       </c>
-      <c r="F12" s="68">
-        <v>-20</v>
+      <c r="F12" s="43">
+        <v>23</v>
       </c>
       <c r="G12" s="42" t="s">
         <v>8</v>
@@ -4200,8 +4247,8 @@
       <c r="E13" s="41">
         <v>5</v>
       </c>
-      <c r="F13" s="68">
-        <v>-20</v>
+      <c r="F13" s="43">
+        <v>23</v>
       </c>
       <c r="G13" s="42" t="s">
         <v>8</v>
@@ -4257,8 +4304,8 @@
       <c r="E14" s="41">
         <v>0</v>
       </c>
-      <c r="F14" s="68">
-        <v>-20</v>
+      <c r="F14" s="43">
+        <v>23</v>
       </c>
       <c r="G14" s="42" t="s">
         <v>8</v>
@@ -4314,8 +4361,8 @@
       <c r="E15" s="41">
         <v>0</v>
       </c>
-      <c r="F15" s="68">
-        <v>-20</v>
+      <c r="F15" s="43">
+        <v>23</v>
       </c>
       <c r="G15" s="42" t="s">
         <v>8</v>
@@ -4371,8 +4418,8 @@
       <c r="E16" s="41">
         <v>24</v>
       </c>
-      <c r="F16" s="68">
-        <v>-20</v>
+      <c r="F16" s="43">
+        <v>23</v>
       </c>
       <c r="G16" s="42" t="s">
         <v>8</v>
@@ -4428,8 +4475,8 @@
       <c r="E17" s="41">
         <v>0</v>
       </c>
-      <c r="F17" s="68">
-        <v>-20</v>
+      <c r="F17" s="43">
+        <v>23</v>
       </c>
       <c r="G17" s="42" t="s">
         <v>8</v>
@@ -4485,8 +4532,8 @@
       <c r="E18" s="41">
         <v>0</v>
       </c>
-      <c r="F18" s="68">
-        <v>-20</v>
+      <c r="F18" s="43">
+        <v>23</v>
       </c>
       <c r="G18" s="42" t="s">
         <v>8</v>
@@ -4542,8 +4589,8 @@
       <c r="E19" s="41">
         <v>99</v>
       </c>
-      <c r="F19" s="68">
-        <v>-20</v>
+      <c r="F19" s="43">
+        <v>23</v>
       </c>
       <c r="G19" s="42" t="s">
         <v>8</v>
@@ -4599,8 +4646,8 @@
       <c r="E20" s="44">
         <v>0</v>
       </c>
-      <c r="F20" s="68">
-        <v>-20</v>
+      <c r="F20" s="46">
+        <v>23</v>
       </c>
       <c r="G20" s="45" t="s">
         <v>9</v>
@@ -4656,8 +4703,8 @@
       <c r="E21" s="44">
         <v>0</v>
       </c>
-      <c r="F21" s="68">
-        <v>-20</v>
+      <c r="F21" s="46">
+        <v>23</v>
       </c>
       <c r="G21" s="45" t="s">
         <v>9</v>
@@ -4713,8 +4760,8 @@
       <c r="E22" s="44">
         <v>5</v>
       </c>
-      <c r="F22" s="68">
-        <v>-20</v>
+      <c r="F22" s="46">
+        <v>23</v>
       </c>
       <c r="G22" s="45" t="s">
         <v>9</v>
@@ -4770,8 +4817,8 @@
       <c r="E23" s="44">
         <v>0</v>
       </c>
-      <c r="F23" s="68">
-        <v>-20</v>
+      <c r="F23" s="46">
+        <v>23</v>
       </c>
       <c r="G23" s="45" t="s">
         <v>9</v>
@@ -4827,8 +4874,8 @@
       <c r="E24" s="44">
         <v>0</v>
       </c>
-      <c r="F24" s="68">
-        <v>-20</v>
+      <c r="F24" s="46">
+        <v>23</v>
       </c>
       <c r="G24" s="45" t="s">
         <v>9</v>
@@ -4884,8 +4931,8 @@
       <c r="E25" s="44">
         <v>24</v>
       </c>
-      <c r="F25" s="68">
-        <v>-20</v>
+      <c r="F25" s="46">
+        <v>23</v>
       </c>
       <c r="G25" s="45" t="s">
         <v>9</v>
@@ -4941,8 +4988,8 @@
       <c r="E26" s="44">
         <v>0</v>
       </c>
-      <c r="F26" s="68">
-        <v>-20</v>
+      <c r="F26" s="46">
+        <v>23</v>
       </c>
       <c r="G26" s="45" t="s">
         <v>9</v>
@@ -4998,8 +5045,8 @@
       <c r="E27" s="44">
         <v>0</v>
       </c>
-      <c r="F27" s="68">
-        <v>-20</v>
+      <c r="F27" s="46">
+        <v>23</v>
       </c>
       <c r="G27" s="45" t="s">
         <v>9</v>
@@ -5055,8 +5102,8 @@
       <c r="E28" s="44">
         <v>99</v>
       </c>
-      <c r="F28" s="68">
-        <v>-20</v>
+      <c r="F28" s="46">
+        <v>23</v>
       </c>
       <c r="G28" s="45" t="s">
         <v>9</v>
@@ -5108,7 +5155,7 @@
   <dimension ref="A1:R60"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5117,7 +5164,7 @@
     <col min="3" max="3" width="18.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="3"/>
     <col min="5" max="5" width="9.140625" style="2"/>
-    <col min="6" max="6" width="10.85546875" style="69" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="17.85546875" customWidth="1"/>
     <col min="8" max="8" width="15.5703125" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
@@ -5148,44 +5195,44 @@
       <c r="E1" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="67" t="s">
-        <v>5</v>
+      <c r="F1" s="49" t="s">
+        <v>10</v>
       </c>
       <c r="G1" s="37" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="37" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I1" s="37" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J1" s="37" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K1" s="37" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L1" s="37" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="M1" s="37" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="N1" s="37" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="O1" s="37" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="P1" s="37" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="Q1" s="37" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="R1" s="50" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -5204,8 +5251,8 @@
       <c r="E2" s="64">
         <v>0</v>
       </c>
-      <c r="F2" s="68">
-        <v>-20</v>
+      <c r="F2" s="65">
+        <v>23</v>
       </c>
       <c r="G2" s="54" t="s">
         <v>7</v>
@@ -5261,8 +5308,8 @@
       <c r="E3" s="64">
         <v>0</v>
       </c>
-      <c r="F3" s="68">
-        <v>-20</v>
+      <c r="F3" s="65">
+        <v>23</v>
       </c>
       <c r="G3" s="54" t="s">
         <v>7</v>
@@ -5318,8 +5365,8 @@
       <c r="E4" s="64">
         <v>5</v>
       </c>
-      <c r="F4" s="68">
-        <v>-20</v>
+      <c r="F4" s="65">
+        <v>23</v>
       </c>
       <c r="G4" s="54" t="s">
         <v>7</v>
@@ -5375,8 +5422,8 @@
       <c r="E5" s="64">
         <v>0</v>
       </c>
-      <c r="F5" s="68">
-        <v>-20</v>
+      <c r="F5" s="65">
+        <v>23</v>
       </c>
       <c r="G5" s="54" t="s">
         <v>7</v>
@@ -5432,8 +5479,8 @@
       <c r="E6" s="64">
         <v>0</v>
       </c>
-      <c r="F6" s="68">
-        <v>-20</v>
+      <c r="F6" s="65">
+        <v>23</v>
       </c>
       <c r="G6" s="54" t="s">
         <v>7</v>
@@ -5489,8 +5536,8 @@
       <c r="E7" s="64">
         <v>24</v>
       </c>
-      <c r="F7" s="68">
-        <v>-20</v>
+      <c r="F7" s="65">
+        <v>23</v>
       </c>
       <c r="G7" s="54" t="s">
         <v>7</v>
@@ -5546,8 +5593,8 @@
       <c r="E8" s="64">
         <v>0</v>
       </c>
-      <c r="F8" s="68">
-        <v>-20</v>
+      <c r="F8" s="65">
+        <v>23</v>
       </c>
       <c r="G8" s="54" t="s">
         <v>7</v>
@@ -5603,8 +5650,8 @@
       <c r="E9" s="64">
         <v>0</v>
       </c>
-      <c r="F9" s="68">
-        <v>-20</v>
+      <c r="F9" s="65">
+        <v>23</v>
       </c>
       <c r="G9" s="54" t="s">
         <v>7</v>
@@ -5660,8 +5707,8 @@
       <c r="E10" s="64">
         <v>49</v>
       </c>
-      <c r="F10" s="68">
-        <v>-20</v>
+      <c r="F10" s="65">
+        <v>23</v>
       </c>
       <c r="G10" s="54" t="s">
         <v>7</v>
@@ -5717,8 +5764,8 @@
       <c r="E11" s="64">
         <v>0</v>
       </c>
-      <c r="F11" s="68">
-        <v>-20</v>
+      <c r="F11" s="65">
+        <v>23</v>
       </c>
       <c r="G11" s="54" t="s">
         <v>8</v>
@@ -5774,8 +5821,8 @@
       <c r="E12" s="64">
         <v>0</v>
       </c>
-      <c r="F12" s="68">
-        <v>-20</v>
+      <c r="F12" s="65">
+        <v>23</v>
       </c>
       <c r="G12" s="54" t="s">
         <v>8</v>
@@ -5831,8 +5878,8 @@
       <c r="E13" s="64">
         <v>5</v>
       </c>
-      <c r="F13" s="68">
-        <v>-20</v>
+      <c r="F13" s="65">
+        <v>23</v>
       </c>
       <c r="G13" s="54" t="s">
         <v>8</v>
@@ -5888,8 +5935,8 @@
       <c r="E14" s="64">
         <v>0</v>
       </c>
-      <c r="F14" s="68">
-        <v>-20</v>
+      <c r="F14" s="65">
+        <v>23</v>
       </c>
       <c r="G14" s="54" t="s">
         <v>8</v>
@@ -5945,8 +5992,8 @@
       <c r="E15" s="64">
         <v>0</v>
       </c>
-      <c r="F15" s="68">
-        <v>-20</v>
+      <c r="F15" s="65">
+        <v>23</v>
       </c>
       <c r="G15" s="54" t="s">
         <v>8</v>
@@ -6002,8 +6049,8 @@
       <c r="E16" s="64">
         <v>24</v>
       </c>
-      <c r="F16" s="68">
-        <v>-20</v>
+      <c r="F16" s="65">
+        <v>23</v>
       </c>
       <c r="G16" s="54" t="s">
         <v>8</v>
@@ -6059,8 +6106,8 @@
       <c r="E17" s="64">
         <v>0</v>
       </c>
-      <c r="F17" s="68">
-        <v>-20</v>
+      <c r="F17" s="65">
+        <v>23</v>
       </c>
       <c r="G17" s="54" t="s">
         <v>8</v>
@@ -6116,8 +6163,8 @@
       <c r="E18" s="64">
         <v>0</v>
       </c>
-      <c r="F18" s="68">
-        <v>-20</v>
+      <c r="F18" s="65">
+        <v>23</v>
       </c>
       <c r="G18" s="54" t="s">
         <v>8</v>
@@ -6173,8 +6220,8 @@
       <c r="E19" s="64">
         <v>49</v>
       </c>
-      <c r="F19" s="68">
-        <v>-20</v>
+      <c r="F19" s="65">
+        <v>23</v>
       </c>
       <c r="G19" s="54" t="s">
         <v>8</v>
@@ -6230,8 +6277,8 @@
       <c r="E20" s="64">
         <v>0</v>
       </c>
-      <c r="F20" s="68">
-        <v>-20</v>
+      <c r="F20" s="65">
+        <v>23</v>
       </c>
       <c r="G20" s="54" t="s">
         <v>9</v>
@@ -6287,8 +6334,8 @@
       <c r="E21" s="64">
         <v>0</v>
       </c>
-      <c r="F21" s="68">
-        <v>-20</v>
+      <c r="F21" s="65">
+        <v>23</v>
       </c>
       <c r="G21" s="54" t="s">
         <v>9</v>
@@ -6344,8 +6391,8 @@
       <c r="E22" s="64">
         <v>5</v>
       </c>
-      <c r="F22" s="68">
-        <v>-20</v>
+      <c r="F22" s="65">
+        <v>23</v>
       </c>
       <c r="G22" s="54" t="s">
         <v>9</v>
@@ -6401,8 +6448,8 @@
       <c r="E23" s="64">
         <v>0</v>
       </c>
-      <c r="F23" s="68">
-        <v>-20</v>
+      <c r="F23" s="65">
+        <v>23</v>
       </c>
       <c r="G23" s="54" t="s">
         <v>9</v>
@@ -6458,8 +6505,8 @@
       <c r="E24" s="64">
         <v>0</v>
       </c>
-      <c r="F24" s="68">
-        <v>-20</v>
+      <c r="F24" s="65">
+        <v>23</v>
       </c>
       <c r="G24" s="54" t="s">
         <v>9</v>
@@ -6515,8 +6562,8 @@
       <c r="E25" s="64">
         <v>24</v>
       </c>
-      <c r="F25" s="68">
-        <v>-20</v>
+      <c r="F25" s="65">
+        <v>23</v>
       </c>
       <c r="G25" s="54" t="s">
         <v>9</v>
@@ -6572,8 +6619,8 @@
       <c r="E26" s="64">
         <v>0</v>
       </c>
-      <c r="F26" s="68">
-        <v>-20</v>
+      <c r="F26" s="65">
+        <v>23</v>
       </c>
       <c r="G26" s="54" t="s">
         <v>9</v>
@@ -6629,8 +6676,8 @@
       <c r="E27" s="64">
         <v>0</v>
       </c>
-      <c r="F27" s="68">
-        <v>-20</v>
+      <c r="F27" s="65">
+        <v>23</v>
       </c>
       <c r="G27" s="54" t="s">
         <v>9</v>
@@ -6686,8 +6733,8 @@
       <c r="E28" s="64">
         <v>49</v>
       </c>
-      <c r="F28" s="68">
-        <v>-20</v>
+      <c r="F28" s="65">
+        <v>23</v>
       </c>
       <c r="G28" s="54" t="s">
         <v>9</v>
@@ -6746,7 +6793,7 @@
     </row>
     <row r="60" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J60" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -6763,8 +6810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D108741B-A8D0-4BB3-B12C-6B68B68001DF}">
   <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection sqref="A1:R28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6773,12 +6820,12 @@
     <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="69" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
     <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.85546875" customWidth="1"/>
     <col min="10" max="10" width="14.85546875" customWidth="1"/>
-    <col min="11" max="11" width="18.42578125" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" customWidth="1"/>
     <col min="12" max="12" width="17.140625" customWidth="1"/>
     <col min="13" max="13" width="14.42578125" customWidth="1"/>
     <col min="14" max="14" width="15.28515625" customWidth="1"/>
@@ -6804,44 +6851,44 @@
       <c r="E1" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="67" t="s">
+      <c r="F1" s="62" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="61" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="37" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I1" s="37" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J1" s="37" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K1" s="37" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L1" s="37" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="M1" s="37" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="N1" s="37" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="O1" s="37" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="P1" s="37" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="Q1" s="37" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="R1" s="50" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -6860,8 +6907,8 @@
       <c r="E2" s="51">
         <v>0</v>
       </c>
-      <c r="F2" s="68">
-        <v>-20</v>
+      <c r="F2" s="52">
+        <v>23</v>
       </c>
       <c r="G2" s="39" t="s">
         <v>7</v>
@@ -6917,8 +6964,8 @@
       <c r="E3" s="51">
         <v>0</v>
       </c>
-      <c r="F3" s="68">
-        <v>-20</v>
+      <c r="F3" s="52">
+        <v>23</v>
       </c>
       <c r="G3" s="39" t="s">
         <v>7</v>
@@ -6974,8 +7021,8 @@
       <c r="E4" s="51">
         <v>5</v>
       </c>
-      <c r="F4" s="68">
-        <v>-20</v>
+      <c r="F4" s="52">
+        <v>23</v>
       </c>
       <c r="G4" s="39" t="s">
         <v>7</v>
@@ -7031,8 +7078,8 @@
       <c r="E5" s="51">
         <v>0</v>
       </c>
-      <c r="F5" s="68">
-        <v>-20</v>
+      <c r="F5" s="52">
+        <v>23</v>
       </c>
       <c r="G5" s="39" t="s">
         <v>7</v>
@@ -7088,8 +7135,8 @@
       <c r="E6" s="51">
         <v>0</v>
       </c>
-      <c r="F6" s="68">
-        <v>-20</v>
+      <c r="F6" s="52">
+        <v>23</v>
       </c>
       <c r="G6" s="39" t="s">
         <v>7</v>
@@ -7145,8 +7192,8 @@
       <c r="E7" s="51">
         <v>24</v>
       </c>
-      <c r="F7" s="68">
-        <v>-20</v>
+      <c r="F7" s="52">
+        <v>23</v>
       </c>
       <c r="G7" s="39" t="s">
         <v>7</v>
@@ -7202,8 +7249,8 @@
       <c r="E8" s="51">
         <v>0</v>
       </c>
-      <c r="F8" s="68">
-        <v>-20</v>
+      <c r="F8" s="52">
+        <v>23</v>
       </c>
       <c r="G8" s="39" t="s">
         <v>7</v>
@@ -7259,8 +7306,8 @@
       <c r="E9" s="51">
         <v>0</v>
       </c>
-      <c r="F9" s="68">
-        <v>-20</v>
+      <c r="F9" s="52">
+        <v>23</v>
       </c>
       <c r="G9" s="39" t="s">
         <v>7</v>
@@ -7316,8 +7363,8 @@
       <c r="E10" s="51">
         <v>49</v>
       </c>
-      <c r="F10" s="68">
-        <v>-20</v>
+      <c r="F10" s="52">
+        <v>23</v>
       </c>
       <c r="G10" s="39" t="s">
         <v>7</v>
@@ -7373,8 +7420,8 @@
       <c r="E11" s="41">
         <v>0</v>
       </c>
-      <c r="F11" s="68">
-        <v>-20</v>
+      <c r="F11" s="43">
+        <v>23</v>
       </c>
       <c r="G11" s="42" t="s">
         <v>8</v>
@@ -7430,8 +7477,8 @@
       <c r="E12" s="41">
         <v>0</v>
       </c>
-      <c r="F12" s="68">
-        <v>-20</v>
+      <c r="F12" s="43">
+        <v>23</v>
       </c>
       <c r="G12" s="42" t="s">
         <v>8</v>
@@ -7487,8 +7534,8 @@
       <c r="E13" s="41">
         <v>5</v>
       </c>
-      <c r="F13" s="68">
-        <v>-20</v>
+      <c r="F13" s="43">
+        <v>23</v>
       </c>
       <c r="G13" s="42" t="s">
         <v>8</v>
@@ -7544,8 +7591,8 @@
       <c r="E14" s="41">
         <v>0</v>
       </c>
-      <c r="F14" s="68">
-        <v>-20</v>
+      <c r="F14" s="43">
+        <v>23</v>
       </c>
       <c r="G14" s="42" t="s">
         <v>8</v>
@@ -7601,8 +7648,8 @@
       <c r="E15" s="41">
         <v>0</v>
       </c>
-      <c r="F15" s="68">
-        <v>-20</v>
+      <c r="F15" s="43">
+        <v>23</v>
       </c>
       <c r="G15" s="42" t="s">
         <v>8</v>
@@ -7658,8 +7705,8 @@
       <c r="E16" s="41">
         <v>24</v>
       </c>
-      <c r="F16" s="68">
-        <v>-20</v>
+      <c r="F16" s="43">
+        <v>23</v>
       </c>
       <c r="G16" s="42" t="s">
         <v>8</v>
@@ -7715,8 +7762,8 @@
       <c r="E17" s="41">
         <v>0</v>
       </c>
-      <c r="F17" s="68">
-        <v>-20</v>
+      <c r="F17" s="43">
+        <v>23</v>
       </c>
       <c r="G17" s="42" t="s">
         <v>8</v>
@@ -7772,8 +7819,8 @@
       <c r="E18" s="41">
         <v>0</v>
       </c>
-      <c r="F18" s="68">
-        <v>-20</v>
+      <c r="F18" s="43">
+        <v>23</v>
       </c>
       <c r="G18" s="42" t="s">
         <v>8</v>
@@ -7829,8 +7876,8 @@
       <c r="E19" s="41">
         <v>49</v>
       </c>
-      <c r="F19" s="68">
-        <v>-20</v>
+      <c r="F19" s="43">
+        <v>23</v>
       </c>
       <c r="G19" s="42" t="s">
         <v>8</v>
@@ -7886,8 +7933,8 @@
       <c r="E20" s="44">
         <v>0</v>
       </c>
-      <c r="F20" s="68">
-        <v>-20</v>
+      <c r="F20" s="46">
+        <v>23</v>
       </c>
       <c r="G20" s="45" t="s">
         <v>9</v>
@@ -7943,8 +7990,8 @@
       <c r="E21" s="44">
         <v>0</v>
       </c>
-      <c r="F21" s="68">
-        <v>-20</v>
+      <c r="F21" s="46">
+        <v>23</v>
       </c>
       <c r="G21" s="45" t="s">
         <v>9</v>
@@ -8000,8 +8047,8 @@
       <c r="E22" s="44">
         <v>5</v>
       </c>
-      <c r="F22" s="68">
-        <v>-20</v>
+      <c r="F22" s="46">
+        <v>23</v>
       </c>
       <c r="G22" s="45" t="s">
         <v>9</v>
@@ -8057,8 +8104,8 @@
       <c r="E23" s="44">
         <v>0</v>
       </c>
-      <c r="F23" s="68">
-        <v>-20</v>
+      <c r="F23" s="46">
+        <v>23</v>
       </c>
       <c r="G23" s="45" t="s">
         <v>9</v>
@@ -8114,8 +8161,8 @@
       <c r="E24" s="44">
         <v>0</v>
       </c>
-      <c r="F24" s="68">
-        <v>-20</v>
+      <c r="F24" s="46">
+        <v>23</v>
       </c>
       <c r="G24" s="45" t="s">
         <v>9</v>
@@ -8171,8 +8218,8 @@
       <c r="E25" s="44">
         <v>24</v>
       </c>
-      <c r="F25" s="68">
-        <v>-20</v>
+      <c r="F25" s="46">
+        <v>23</v>
       </c>
       <c r="G25" s="45" t="s">
         <v>9</v>
@@ -8228,8 +8275,8 @@
       <c r="E26" s="44">
         <v>0</v>
       </c>
-      <c r="F26" s="68">
-        <v>-20</v>
+      <c r="F26" s="46">
+        <v>23</v>
       </c>
       <c r="G26" s="45" t="s">
         <v>9</v>
@@ -8285,8 +8332,8 @@
       <c r="E27" s="44">
         <v>0</v>
       </c>
-      <c r="F27" s="68">
-        <v>-20</v>
+      <c r="F27" s="46">
+        <v>23</v>
       </c>
       <c r="G27" s="45" t="s">
         <v>9</v>
@@ -8342,8 +8389,8 @@
       <c r="E28" s="44">
         <v>49</v>
       </c>
-      <c r="F28" s="68">
-        <v>-20</v>
+      <c r="F28" s="46">
+        <v>23</v>
       </c>
       <c r="G28" s="45" t="s">
         <v>9</v>
@@ -8394,8 +8441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDABD784-AD31-46F2-99DC-A4DD1B41AE1B}">
   <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8403,7 +8450,7 @@
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" style="69" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
     <col min="7" max="7" width="12.140625" customWidth="1"/>
     <col min="8" max="8" width="17.28515625" customWidth="1"/>
     <col min="9" max="9" width="18.140625" customWidth="1"/>
@@ -8434,44 +8481,44 @@
       <c r="E1" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="67" t="s">
+      <c r="F1" s="49" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="37" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="37" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I1" s="37" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J1" s="37" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K1" s="37" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L1" s="37" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="M1" s="37" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="N1" s="37" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="O1" s="37" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="P1" s="37" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="Q1" s="37" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="R1" s="50" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -8490,8 +8537,8 @@
       <c r="E2" s="51">
         <v>0</v>
       </c>
-      <c r="F2" s="68">
-        <v>-20</v>
+      <c r="F2" s="52">
+        <v>23</v>
       </c>
       <c r="G2" s="39" t="s">
         <v>7</v>
@@ -8547,8 +8594,8 @@
       <c r="E3" s="51">
         <v>0</v>
       </c>
-      <c r="F3" s="68">
-        <v>-20</v>
+      <c r="F3" s="52">
+        <v>23</v>
       </c>
       <c r="G3" s="39" t="s">
         <v>7</v>
@@ -8604,8 +8651,8 @@
       <c r="E4" s="51">
         <v>24</v>
       </c>
-      <c r="F4" s="68">
-        <v>-20</v>
+      <c r="F4" s="52">
+        <v>23</v>
       </c>
       <c r="G4" s="39" t="s">
         <v>7</v>
@@ -8661,8 +8708,8 @@
       <c r="E5" s="51">
         <v>0</v>
       </c>
-      <c r="F5" s="68">
-        <v>-20</v>
+      <c r="F5" s="52">
+        <v>23</v>
       </c>
       <c r="G5" s="39" t="s">
         <v>8</v>
@@ -8718,8 +8765,8 @@
       <c r="E6" s="51">
         <v>0</v>
       </c>
-      <c r="F6" s="68">
-        <v>-20</v>
+      <c r="F6" s="52">
+        <v>23</v>
       </c>
       <c r="G6" s="39" t="s">
         <v>8</v>
@@ -8775,8 +8822,8 @@
       <c r="E7" s="51">
         <v>24</v>
       </c>
-      <c r="F7" s="68">
-        <v>-20</v>
+      <c r="F7" s="52">
+        <v>23</v>
       </c>
       <c r="G7" s="39" t="s">
         <v>8</v>
@@ -8832,8 +8879,8 @@
       <c r="E8" s="51">
         <v>0</v>
       </c>
-      <c r="F8" s="68">
-        <v>-20</v>
+      <c r="F8" s="52">
+        <v>23</v>
       </c>
       <c r="G8" s="39" t="s">
         <v>9</v>
@@ -8889,8 +8936,8 @@
       <c r="E9" s="51">
         <v>0</v>
       </c>
-      <c r="F9" s="68">
-        <v>-20</v>
+      <c r="F9" s="52">
+        <v>23</v>
       </c>
       <c r="G9" s="39" t="s">
         <v>9</v>
@@ -8946,8 +8993,8 @@
       <c r="E10" s="51">
         <v>24</v>
       </c>
-      <c r="F10" s="68">
-        <v>-20</v>
+      <c r="F10" s="52">
+        <v>23</v>
       </c>
       <c r="G10" s="39" t="s">
         <v>9</v>
@@ -9003,8 +9050,8 @@
       <c r="E11" s="41">
         <v>0</v>
       </c>
-      <c r="F11" s="68">
-        <v>-20</v>
+      <c r="F11" s="52">
+        <v>23</v>
       </c>
       <c r="G11" s="42" t="s">
         <v>8</v>
@@ -9060,8 +9107,8 @@
       <c r="E12" s="41">
         <v>0</v>
       </c>
-      <c r="F12" s="68">
-        <v>-20</v>
+      <c r="F12" s="52">
+        <v>23</v>
       </c>
       <c r="G12" s="42" t="s">
         <v>8</v>
@@ -9117,8 +9164,8 @@
       <c r="E13" s="41">
         <v>49</v>
       </c>
-      <c r="F13" s="68">
-        <v>-20</v>
+      <c r="F13" s="52">
+        <v>23</v>
       </c>
       <c r="G13" s="42" t="s">
         <v>8</v>
@@ -9168,10 +9215,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F7206B6-36E5-4637-B4E1-0FEA65E91330}">
-  <dimension ref="A1:T28"/>
+  <dimension ref="A1:U28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="T10" sqref="T10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9179,16 +9226,15 @@
     <col min="2" max="2" width="10.85546875" customWidth="1"/>
     <col min="3" max="3" width="14.140625" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="69" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1"/>
     <col min="7" max="7" width="16.5703125" customWidth="1"/>
     <col min="8" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.5703125" customWidth="1"/>
     <col min="13" max="17" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
@@ -9204,47 +9250,53 @@
       <c r="E1" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="67" t="s">
+      <c r="F1" s="49" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="37" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="37" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I1" s="37" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J1" s="37" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K1" s="37" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L1" s="37" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="M1" s="37" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="N1" s="37" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="O1" s="37" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="P1" s="37" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="Q1" s="37" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="R1" s="50" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="T1" s="69" t="s">
+        <v>89</v>
+      </c>
+      <c r="U1" s="69" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="51">
         <v>66</v>
       </c>
@@ -9260,7 +9312,7 @@
       <c r="E2" s="51">
         <v>0</v>
       </c>
-      <c r="F2" s="68">
+      <c r="F2" s="70">
         <v>-20</v>
       </c>
       <c r="G2" s="39" t="s">
@@ -9278,8 +9330,9 @@
       <c r="K2" s="39">
         <v>1000000000</v>
       </c>
-      <c r="L2" s="2">
-        <v>1719199999.9999998</v>
+      <c r="L2" s="53">
+        <f>((R2+'Frequency Range Setting'!$B$2)*1000000)+$U$2</f>
+        <v>1714699999.9999998</v>
       </c>
       <c r="M2" s="39">
         <v>150000</v>
@@ -9290,8 +9343,9 @@
       <c r="O2" s="54">
         <v>1000000000</v>
       </c>
-      <c r="P2" s="2">
-        <v>1702199999.9999998</v>
+      <c r="P2" s="53">
+        <f>((R2-'Frequency Range Setting'!$B$2)*1000000)-$U$2</f>
+        <v>1706699999.9999998</v>
       </c>
       <c r="Q2" s="39">
         <v>12750000000</v>
@@ -9301,10 +9355,14 @@
         <v>1710.6999999999998</v>
       </c>
       <c r="T2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+        <v>1000000</v>
+      </c>
+      <c r="U2">
+        <f>T2/2</f>
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="51"/>
       <c r="B3" s="39">
         <v>1.4</v>
@@ -9318,7 +9376,7 @@
       <c r="E3" s="51">
         <v>0</v>
       </c>
-      <c r="F3" s="68">
+      <c r="F3" s="70">
         <v>-20</v>
       </c>
       <c r="G3" s="39" t="s">
@@ -9337,8 +9395,8 @@
         <v>1000000000</v>
       </c>
       <c r="L3" s="53">
-        <f>(R3+'Frequency Range Setting'!$B$2)*1000000</f>
-        <v>1714199999.9999998</v>
+        <f>((R3+'Frequency Range Setting'!$B$2)*1000000)+$U$2</f>
+        <v>1714699999.9999998</v>
       </c>
       <c r="M3" s="39">
         <v>150000</v>
@@ -9350,8 +9408,8 @@
         <v>1000000000</v>
       </c>
       <c r="P3" s="53">
-        <f>(R3-'Frequency Range Setting'!$B$2)*1000000</f>
-        <v>1707199999.9999998</v>
+        <f>((R3-'Frequency Range Setting'!$B$2)*1000000)-$U$2</f>
+        <v>1706699999.9999998</v>
       </c>
       <c r="Q3" s="39">
         <v>12750000000</v>
@@ -9360,11 +9418,8 @@
         <f t="shared" ref="R3:R28" si="0">C3-400</f>
         <v>1710.6999999999998</v>
       </c>
-      <c r="T3" s="2">
-        <v>1702199999.9999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="51"/>
       <c r="B4" s="39">
         <v>1.4</v>
@@ -9378,7 +9433,7 @@
       <c r="E4" s="51">
         <v>5</v>
       </c>
-      <c r="F4" s="68">
+      <c r="F4" s="70">
         <v>-20</v>
       </c>
       <c r="G4" s="39" t="s">
@@ -9397,8 +9452,8 @@
         <v>1000000000</v>
       </c>
       <c r="L4" s="53">
-        <f>(R4+'Frequency Range Setting'!$B$2)*1000000</f>
-        <v>1714199999.9999998</v>
+        <f>((R4+'Frequency Range Setting'!$B$2)*1000000)+$U$2</f>
+        <v>1714699999.9999998</v>
       </c>
       <c r="M4" s="39">
         <v>150000</v>
@@ -9410,8 +9465,8 @@
         <v>1000000000</v>
       </c>
       <c r="P4" s="53">
-        <f>(R4-'Frequency Range Setting'!$B$2)*1000000</f>
-        <v>1707199999.9999998</v>
+        <f>((R4-'Frequency Range Setting'!$B$2)*1000000)-$U$2</f>
+        <v>1706699999.9999998</v>
       </c>
       <c r="Q4" s="39">
         <v>12750000000</v>
@@ -9420,11 +9475,8 @@
         <f t="shared" si="0"/>
         <v>1710.6999999999998</v>
       </c>
-      <c r="T4">
-        <v>10000000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="51"/>
       <c r="B5" s="39">
         <v>5</v>
@@ -9438,7 +9490,7 @@
       <c r="E5" s="51">
         <v>0</v>
       </c>
-      <c r="F5" s="68">
+      <c r="F5" s="70">
         <v>-20</v>
       </c>
       <c r="G5" s="39" t="s">
@@ -9457,8 +9509,8 @@
         <v>1000000000</v>
       </c>
       <c r="L5" s="53">
-        <f>(R5+'Frequency Range Setting'!$B$4)*1000000</f>
-        <v>1725000000</v>
+        <f>((R5+'Frequency Range Setting'!$B$4)*1000000)+$U$2</f>
+        <v>1725500000</v>
       </c>
       <c r="M5" s="39">
         <v>150000</v>
@@ -9470,8 +9522,8 @@
         <v>1000000000</v>
       </c>
       <c r="P5" s="58">
-        <f>(R5-'Frequency Range Setting'!$B$4)*1000000</f>
-        <v>1700000000</v>
+        <f>((R5-'Frequency Range Setting'!$B$4)*1000000)-$U$2</f>
+        <v>1699500000</v>
       </c>
       <c r="Q5" s="39">
         <v>12750000000</v>
@@ -9480,11 +9532,8 @@
         <f t="shared" si="0"/>
         <v>1712.5</v>
       </c>
-      <c r="T5" s="2">
-        <v>1719199999.9999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="51"/>
       <c r="B6" s="39">
         <v>5</v>
@@ -9498,7 +9547,7 @@
       <c r="E6" s="51">
         <v>0</v>
       </c>
-      <c r="F6" s="68">
+      <c r="F6" s="70">
         <v>-20</v>
       </c>
       <c r="G6" s="39" t="s">
@@ -9517,8 +9566,8 @@
         <v>1000000000</v>
       </c>
       <c r="L6" s="53">
-        <f>(R6+'Frequency Range Setting'!$B$4)*1000000</f>
-        <v>1725000000</v>
+        <f>((R6+'Frequency Range Setting'!$B$4)*1000000)+$U$2</f>
+        <v>1725500000</v>
       </c>
       <c r="M6" s="39">
         <v>150000</v>
@@ -9530,8 +9579,8 @@
         <v>1000000000</v>
       </c>
       <c r="P6" s="58">
-        <f>(R6-'Frequency Range Setting'!$B$4)*1000000</f>
-        <v>1700000000</v>
+        <f>((R6-'Frequency Range Setting'!$B$4)*1000000)-$U$2</f>
+        <v>1699500000</v>
       </c>
       <c r="Q6" s="39">
         <v>12750000000</v>
@@ -9540,12 +9589,8 @@
         <f t="shared" si="0"/>
         <v>1712.5</v>
       </c>
-      <c r="T6">
-        <f>T4/2</f>
-        <v>5000000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="51"/>
       <c r="B7" s="39">
         <v>5</v>
@@ -9559,7 +9604,7 @@
       <c r="E7" s="51">
         <v>24</v>
       </c>
-      <c r="F7" s="68">
+      <c r="F7" s="70">
         <v>-20</v>
       </c>
       <c r="G7" s="39" t="s">
@@ -9578,8 +9623,8 @@
         <v>1000000000</v>
       </c>
       <c r="L7" s="53">
-        <f>(R7+'Frequency Range Setting'!$B$4)*1000000</f>
-        <v>1725000000</v>
+        <f>((R7+'Frequency Range Setting'!$B$4)*1000000)+$U$2</f>
+        <v>1725500000</v>
       </c>
       <c r="M7" s="39">
         <v>150000</v>
@@ -9591,8 +9636,8 @@
         <v>1000000000</v>
       </c>
       <c r="P7" s="58">
-        <f>(R7-'Frequency Range Setting'!$B$4)*1000000</f>
-        <v>1700000000</v>
+        <f>((R7-'Frequency Range Setting'!$B$4)*1000000)-$U$2</f>
+        <v>1699500000</v>
       </c>
       <c r="Q7" s="39">
         <v>12750000000</v>
@@ -9602,7 +9647,7 @@
         <v>1712.5</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="51"/>
       <c r="B8" s="39">
         <v>20</v>
@@ -9616,7 +9661,7 @@
       <c r="E8" s="51">
         <v>0</v>
       </c>
-      <c r="F8" s="68">
+      <c r="F8" s="70">
         <v>-20</v>
       </c>
       <c r="G8" s="39" t="s">
@@ -9635,8 +9680,8 @@
         <v>1000000000</v>
       </c>
       <c r="L8" s="53">
-        <f>(R8+'Frequency Range Setting'!$B$7)*1000000</f>
-        <v>1755000000</v>
+        <f>((R8+'Frequency Range Setting'!$B$7)*1000000)+$U$2</f>
+        <v>1755500000</v>
       </c>
       <c r="M8" s="39">
         <v>150000</v>
@@ -9648,8 +9693,8 @@
         <v>1000000000</v>
       </c>
       <c r="P8" s="53">
-        <f>(R8-'Frequency Range Setting'!$B$7)*1000000</f>
-        <v>1685000000</v>
+        <f>((R8-'Frequency Range Setting'!$B$7)*1000000)-$U$2</f>
+        <v>1684500000</v>
       </c>
       <c r="Q8" s="39">
         <v>12750000000</v>
@@ -9659,7 +9704,7 @@
         <v>1720</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="51"/>
       <c r="B9" s="39">
         <v>20</v>
@@ -9673,7 +9718,7 @@
       <c r="E9" s="51">
         <v>0</v>
       </c>
-      <c r="F9" s="68">
+      <c r="F9" s="70">
         <v>-20</v>
       </c>
       <c r="G9" s="39" t="s">
@@ -9692,8 +9737,8 @@
         <v>1000000000</v>
       </c>
       <c r="L9" s="53">
-        <f>(R9+'Frequency Range Setting'!$B$7)*1000000</f>
-        <v>1755000000</v>
+        <f>((R9+'Frequency Range Setting'!$B$7)*1000000)+$U$2</f>
+        <v>1755500000</v>
       </c>
       <c r="M9" s="39">
         <v>150000</v>
@@ -9705,8 +9750,8 @@
         <v>1000000000</v>
       </c>
       <c r="P9" s="53">
-        <f>(R9-'Frequency Range Setting'!$B$7)*1000000</f>
-        <v>1685000000</v>
+        <f>((R9-'Frequency Range Setting'!$B$7)*1000000)-$U$2</f>
+        <v>1684500000</v>
       </c>
       <c r="Q9" s="39">
         <v>12750000000</v>
@@ -9716,7 +9761,7 @@
         <v>1720</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="51"/>
       <c r="B10" s="39">
         <v>20</v>
@@ -9730,7 +9775,7 @@
       <c r="E10" s="51">
         <v>99</v>
       </c>
-      <c r="F10" s="68">
+      <c r="F10" s="70">
         <v>-20</v>
       </c>
       <c r="G10" s="39" t="s">
@@ -9749,8 +9794,8 @@
         <v>1000000000</v>
       </c>
       <c r="L10" s="53">
-        <f>(R10+'Frequency Range Setting'!$B$7)*1000000</f>
-        <v>1755000000</v>
+        <f>((R10+'Frequency Range Setting'!$B$7)*1000000)+$U$2</f>
+        <v>1755500000</v>
       </c>
       <c r="M10" s="39">
         <v>150000</v>
@@ -9762,8 +9807,8 @@
         <v>1000000000</v>
       </c>
       <c r="P10" s="53">
-        <f>(R10-'Frequency Range Setting'!$B$7)*1000000</f>
-        <v>1685000000</v>
+        <f>((R10-'Frequency Range Setting'!$B$7)*1000000)-$U$2</f>
+        <v>1684500000</v>
       </c>
       <c r="Q10" s="39">
         <v>12750000000</v>
@@ -9773,7 +9818,7 @@
         <v>1720</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="41"/>
       <c r="B11" s="42">
         <v>1.4</v>
@@ -9787,7 +9832,7 @@
       <c r="E11" s="41">
         <v>0</v>
       </c>
-      <c r="F11" s="68">
+      <c r="F11" s="70">
         <v>-20</v>
       </c>
       <c r="G11" s="42" t="s">
@@ -9806,8 +9851,8 @@
         <v>1000000000</v>
       </c>
       <c r="L11" s="53">
-        <f>(R11+'Frequency Range Setting'!$B$2)*1000000</f>
-        <v>1748500000</v>
+        <f>((R11+'Frequency Range Setting'!$B$2)*1000000)+$U$2</f>
+        <v>1749000000</v>
       </c>
       <c r="M11" s="39">
         <v>150000</v>
@@ -9819,8 +9864,8 @@
         <v>1000000000</v>
       </c>
       <c r="P11" s="53">
-        <f>(R11-'Frequency Range Setting'!$B$2)*1000000</f>
-        <v>1741500000</v>
+        <f>((R11-'Frequency Range Setting'!$B$2)*1000000)-$U$2</f>
+        <v>1741000000</v>
       </c>
       <c r="Q11" s="39">
         <v>12750000000</v>
@@ -9830,7 +9875,7 @@
         <v>1745</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="41"/>
       <c r="B12" s="42">
         <v>1.4</v>
@@ -9844,7 +9889,7 @@
       <c r="E12" s="41">
         <v>0</v>
       </c>
-      <c r="F12" s="68">
+      <c r="F12" s="70">
         <v>-20</v>
       </c>
       <c r="G12" s="42" t="s">
@@ -9863,8 +9908,8 @@
         <v>1000000000</v>
       </c>
       <c r="L12" s="53">
-        <f>(R12+'Frequency Range Setting'!$B$2)*1000000</f>
-        <v>1748500000</v>
+        <f>((R12+'Frequency Range Setting'!$B$2)*1000000)+$U$2</f>
+        <v>1749000000</v>
       </c>
       <c r="M12" s="39">
         <v>150000</v>
@@ -9876,8 +9921,8 @@
         <v>1000000000</v>
       </c>
       <c r="P12" s="53">
-        <f>(R12-'Frequency Range Setting'!$B$2)*1000000</f>
-        <v>1741500000</v>
+        <f>((R12-'Frequency Range Setting'!$B$2)*1000000)-$U$2</f>
+        <v>1741000000</v>
       </c>
       <c r="Q12" s="39">
         <v>12750000000</v>
@@ -9887,7 +9932,7 @@
         <v>1745</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="41"/>
       <c r="B13" s="42">
         <v>1.4</v>
@@ -9901,7 +9946,7 @@
       <c r="E13" s="41">
         <v>5</v>
       </c>
-      <c r="F13" s="68">
+      <c r="F13" s="70">
         <v>-20</v>
       </c>
       <c r="G13" s="42" t="s">
@@ -9920,8 +9965,8 @@
         <v>1000000000</v>
       </c>
       <c r="L13" s="53">
-        <f>(R13+'Frequency Range Setting'!$B$2)*1000000</f>
-        <v>1748500000</v>
+        <f>((R13+'Frequency Range Setting'!$B$2)*1000000)+$U$2</f>
+        <v>1749000000</v>
       </c>
       <c r="M13" s="39">
         <v>150000</v>
@@ -9933,8 +9978,8 @@
         <v>1000000000</v>
       </c>
       <c r="P13" s="53">
-        <f>(R13-'Frequency Range Setting'!$B$2)*1000000</f>
-        <v>1741500000</v>
+        <f>((R13-'Frequency Range Setting'!$B$2)*1000000)-$U$2</f>
+        <v>1741000000</v>
       </c>
       <c r="Q13" s="39">
         <v>12750000000</v>
@@ -9944,7 +9989,7 @@
         <v>1745</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="41"/>
       <c r="B14" s="42">
         <v>5</v>
@@ -9958,7 +10003,7 @@
       <c r="E14" s="41">
         <v>0</v>
       </c>
-      <c r="F14" s="68">
+      <c r="F14" s="70">
         <v>-20</v>
       </c>
       <c r="G14" s="42" t="s">
@@ -9977,8 +10022,8 @@
         <v>1000000000</v>
       </c>
       <c r="L14" s="53">
-        <f>(R14+'Frequency Range Setting'!$B$4)*1000000</f>
-        <v>1757500000</v>
+        <f>((R14+'Frequency Range Setting'!$B$4)*1000000)+$U$2</f>
+        <v>1758000000</v>
       </c>
       <c r="M14" s="39">
         <v>150000</v>
@@ -9990,8 +10035,8 @@
         <v>1000000000</v>
       </c>
       <c r="P14" s="58">
-        <f>(R14-'Frequency Range Setting'!$B$4)*1000000</f>
-        <v>1732500000</v>
+        <f>((R14-'Frequency Range Setting'!$B$4)*1000000)-$U$2</f>
+        <v>1732000000</v>
       </c>
       <c r="Q14" s="39">
         <v>12750000000</v>
@@ -10001,7 +10046,7 @@
         <v>1745</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="41"/>
       <c r="B15" s="42">
         <v>5</v>
@@ -10015,7 +10060,7 @@
       <c r="E15" s="41">
         <v>0</v>
       </c>
-      <c r="F15" s="68">
+      <c r="F15" s="70">
         <v>-20</v>
       </c>
       <c r="G15" s="42" t="s">
@@ -10034,8 +10079,8 @@
         <v>1000000000</v>
       </c>
       <c r="L15" s="53">
-        <f>(R15+'Frequency Range Setting'!$B$4)*1000000</f>
-        <v>1757500000</v>
+        <f>((R15+'Frequency Range Setting'!$B$4)*1000000)+$U$2</f>
+        <v>1758000000</v>
       </c>
       <c r="M15" s="39">
         <v>150000</v>
@@ -10047,8 +10092,8 @@
         <v>1000000000</v>
       </c>
       <c r="P15" s="58">
-        <f>(R15-'Frequency Range Setting'!$B$4)*1000000</f>
-        <v>1732500000</v>
+        <f>((R15-'Frequency Range Setting'!$B$4)*1000000)-$U$2</f>
+        <v>1732000000</v>
       </c>
       <c r="Q15" s="39">
         <v>12750000000</v>
@@ -10058,7 +10103,7 @@
         <v>1745</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="41"/>
       <c r="B16" s="42">
         <v>5</v>
@@ -10072,7 +10117,7 @@
       <c r="E16" s="41">
         <v>24</v>
       </c>
-      <c r="F16" s="68">
+      <c r="F16" s="70">
         <v>-20</v>
       </c>
       <c r="G16" s="42" t="s">
@@ -10091,8 +10136,8 @@
         <v>1000000000</v>
       </c>
       <c r="L16" s="53">
-        <f>(R16+'Frequency Range Setting'!$B$4)*1000000</f>
-        <v>1757500000</v>
+        <f>((R16+'Frequency Range Setting'!$B$4)*1000000)+$U$2</f>
+        <v>1758000000</v>
       </c>
       <c r="M16" s="39">
         <v>150000</v>
@@ -10104,8 +10149,8 @@
         <v>1000000000</v>
       </c>
       <c r="P16" s="58">
-        <f>(R16-'Frequency Range Setting'!$B$4)*1000000</f>
-        <v>1732500000</v>
+        <f>((R16-'Frequency Range Setting'!$B$4)*1000000)-$U$2</f>
+        <v>1732000000</v>
       </c>
       <c r="Q16" s="39">
         <v>12750000000</v>
@@ -10129,7 +10174,7 @@
       <c r="E17" s="41">
         <v>0</v>
       </c>
-      <c r="F17" s="68">
+      <c r="F17" s="70">
         <v>-20</v>
       </c>
       <c r="G17" s="42" t="s">
@@ -10148,8 +10193,8 @@
         <v>1000000000</v>
       </c>
       <c r="L17" s="53">
-        <f>(R17+'Frequency Range Setting'!$B$7)*1000000</f>
-        <v>1780000000</v>
+        <f>((R17+'Frequency Range Setting'!$B$7)*1000000)+$U$2</f>
+        <v>1780500000</v>
       </c>
       <c r="M17" s="39">
         <v>150000</v>
@@ -10161,8 +10206,8 @@
         <v>1000000000</v>
       </c>
       <c r="P17" s="53">
-        <f>(R17-'Frequency Range Setting'!$B$7)*1000000</f>
-        <v>1710000000</v>
+        <f>((R17-'Frequency Range Setting'!$B$7)*1000000)-$U$2</f>
+        <v>1709500000</v>
       </c>
       <c r="Q17" s="39">
         <v>12750000000</v>
@@ -10186,7 +10231,7 @@
       <c r="E18" s="41">
         <v>0</v>
       </c>
-      <c r="F18" s="68">
+      <c r="F18" s="70">
         <v>-20</v>
       </c>
       <c r="G18" s="42" t="s">
@@ -10205,8 +10250,8 @@
         <v>1000000000</v>
       </c>
       <c r="L18" s="53">
-        <f>(R18+'Frequency Range Setting'!$B$7)*1000000</f>
-        <v>1780000000</v>
+        <f>((R18+'Frequency Range Setting'!$B$7)*1000000)+$U$2</f>
+        <v>1780500000</v>
       </c>
       <c r="M18" s="39">
         <v>150000</v>
@@ -10218,8 +10263,8 @@
         <v>1000000000</v>
       </c>
       <c r="P18" s="53">
-        <f>(R18-'Frequency Range Setting'!$B$7)*1000000</f>
-        <v>1710000000</v>
+        <f>((R18-'Frequency Range Setting'!$B$7)*1000000)-$U$2</f>
+        <v>1709500000</v>
       </c>
       <c r="Q18" s="39">
         <v>12750000000</v>
@@ -10243,7 +10288,7 @@
       <c r="E19" s="41">
         <v>99</v>
       </c>
-      <c r="F19" s="68">
+      <c r="F19" s="70">
         <v>-20</v>
       </c>
       <c r="G19" s="42" t="s">
@@ -10262,8 +10307,8 @@
         <v>1000000000</v>
       </c>
       <c r="L19" s="53">
-        <f>(R19+'Frequency Range Setting'!$B$7)*1000000</f>
-        <v>1780000000</v>
+        <f>((R19+'Frequency Range Setting'!$B$7)*1000000)+$U$2</f>
+        <v>1780500000</v>
       </c>
       <c r="M19" s="39">
         <v>150000</v>
@@ -10275,8 +10320,8 @@
         <v>1000000000</v>
       </c>
       <c r="P19" s="53">
-        <f>(R19-'Frequency Range Setting'!$B$7)*1000000</f>
-        <v>1710000000</v>
+        <f>((R19-'Frequency Range Setting'!$B$7)*1000000)-$U$2</f>
+        <v>1709500000</v>
       </c>
       <c r="Q19" s="39">
         <v>12750000000</v>
@@ -10300,7 +10345,7 @@
       <c r="E20" s="44">
         <v>0</v>
       </c>
-      <c r="F20" s="68">
+      <c r="F20" s="70">
         <v>-20</v>
       </c>
       <c r="G20" s="45" t="s">
@@ -10319,8 +10364,8 @@
         <v>1000000000</v>
       </c>
       <c r="L20" s="53">
-        <f>(R20+'Frequency Range Setting'!$B$2)*1000000</f>
-        <v>1782800000.0000002</v>
+        <f>((R20+'Frequency Range Setting'!$B$2)*1000000)+$U$2</f>
+        <v>1783300000.0000002</v>
       </c>
       <c r="M20" s="39">
         <v>150000</v>
@@ -10332,8 +10377,8 @@
         <v>1000000000</v>
       </c>
       <c r="P20" s="53">
-        <f>(R20-'Frequency Range Setting'!$B$2)*1000000</f>
-        <v>1775800000.0000002</v>
+        <f>((R20-'Frequency Range Setting'!$B$2)*1000000)-$U$2</f>
+        <v>1775300000.0000002</v>
       </c>
       <c r="Q20" s="39">
         <v>12750000000</v>
@@ -10357,7 +10402,7 @@
       <c r="E21" s="44">
         <v>0</v>
       </c>
-      <c r="F21" s="68">
+      <c r="F21" s="70">
         <v>-20</v>
       </c>
       <c r="G21" s="45" t="s">
@@ -10376,8 +10421,8 @@
         <v>1000000000</v>
       </c>
       <c r="L21" s="53">
-        <f>(R21+'Frequency Range Setting'!$B$2)*1000000</f>
-        <v>1782800000.0000002</v>
+        <f>((R21+'Frequency Range Setting'!$B$2)*1000000)+$U$2</f>
+        <v>1783300000.0000002</v>
       </c>
       <c r="M21" s="39">
         <v>150000</v>
@@ -10389,8 +10434,8 @@
         <v>1000000000</v>
       </c>
       <c r="P21" s="53">
-        <f>(R21-'Frequency Range Setting'!$B$2)*1000000</f>
-        <v>1775800000.0000002</v>
+        <f>((R21-'Frequency Range Setting'!$B$2)*1000000)-$U$2</f>
+        <v>1775300000.0000002</v>
       </c>
       <c r="Q21" s="39">
         <v>12750000000</v>
@@ -10414,7 +10459,7 @@
       <c r="E22" s="44">
         <v>5</v>
       </c>
-      <c r="F22" s="68">
+      <c r="F22" s="70">
         <v>-20</v>
       </c>
       <c r="G22" s="45" t="s">
@@ -10433,8 +10478,8 @@
         <v>1000000000</v>
       </c>
       <c r="L22" s="53">
-        <f>(R22+'Frequency Range Setting'!$B$2)*1000000</f>
-        <v>1782800000.0000002</v>
+        <f>((R22+'Frequency Range Setting'!$B$2)*1000000)+$U$2</f>
+        <v>1783300000.0000002</v>
       </c>
       <c r="M22" s="39">
         <v>150000</v>
@@ -10446,8 +10491,8 @@
         <v>1000000000</v>
       </c>
       <c r="P22" s="53">
-        <f>(R22-'Frequency Range Setting'!$B$2)*1000000</f>
-        <v>1775800000.0000002</v>
+        <f>((R22-'Frequency Range Setting'!$B$2)*1000000)-$U$2</f>
+        <v>1775300000.0000002</v>
       </c>
       <c r="Q22" s="39">
         <v>12750000000</v>
@@ -10471,7 +10516,7 @@
       <c r="E23" s="44">
         <v>0</v>
       </c>
-      <c r="F23" s="68">
+      <c r="F23" s="70">
         <v>-20</v>
       </c>
       <c r="G23" s="45" t="s">
@@ -10490,8 +10535,8 @@
         <v>1000000000</v>
       </c>
       <c r="L23" s="53">
-        <f>(R23+'Frequency Range Setting'!$B$4)*1000000</f>
-        <v>1790000000</v>
+        <f>((R23+'Frequency Range Setting'!$B$4)*1000000)+$U$2</f>
+        <v>1790500000</v>
       </c>
       <c r="M23" s="39">
         <v>150000</v>
@@ -10503,8 +10548,8 @@
         <v>1000000000</v>
       </c>
       <c r="P23" s="58">
-        <f>(R23-'Frequency Range Setting'!$B$4)*1000000</f>
-        <v>1765000000</v>
+        <f>((R23-'Frequency Range Setting'!$B$4)*1000000)-$U$2</f>
+        <v>1764500000</v>
       </c>
       <c r="Q23" s="39">
         <v>12750000000</v>
@@ -10528,7 +10573,7 @@
       <c r="E24" s="44">
         <v>0</v>
       </c>
-      <c r="F24" s="68">
+      <c r="F24" s="70">
         <v>-20</v>
       </c>
       <c r="G24" s="45" t="s">
@@ -10547,8 +10592,8 @@
         <v>1000000000</v>
       </c>
       <c r="L24" s="53">
-        <f>(R24+'Frequency Range Setting'!$B$4)*1000000</f>
-        <v>1790000000</v>
+        <f>((R24+'Frequency Range Setting'!$B$4)*1000000)+$U$2</f>
+        <v>1790500000</v>
       </c>
       <c r="M24" s="39">
         <v>150000</v>
@@ -10560,8 +10605,8 @@
         <v>1000000000</v>
       </c>
       <c r="P24" s="58">
-        <f>(R24-'Frequency Range Setting'!$B$4)*1000000</f>
-        <v>1765000000</v>
+        <f>((R24-'Frequency Range Setting'!$B$4)*1000000)-$U$2</f>
+        <v>1764500000</v>
       </c>
       <c r="Q24" s="39">
         <v>12750000000</v>
@@ -10585,7 +10630,7 @@
       <c r="E25" s="44">
         <v>24</v>
       </c>
-      <c r="F25" s="68">
+      <c r="F25" s="70">
         <v>-20</v>
       </c>
       <c r="G25" s="45" t="s">
@@ -10604,8 +10649,8 @@
         <v>1000000000</v>
       </c>
       <c r="L25" s="53">
-        <f>(R25+'Frequency Range Setting'!$B$4)*1000000</f>
-        <v>1790000000</v>
+        <f>((R25+'Frequency Range Setting'!$B$4)*1000000)+$U$2</f>
+        <v>1790500000</v>
       </c>
       <c r="M25" s="39">
         <v>150000</v>
@@ -10617,8 +10662,8 @@
         <v>1000000000</v>
       </c>
       <c r="P25" s="58">
-        <f>(R25-'Frequency Range Setting'!$B$4)*1000000</f>
-        <v>1765000000</v>
+        <f>((R25-'Frequency Range Setting'!$B$4)*1000000)-$U$2</f>
+        <v>1764500000</v>
       </c>
       <c r="Q25" s="39">
         <v>12750000000</v>
@@ -10642,7 +10687,7 @@
       <c r="E26" s="44">
         <v>0</v>
       </c>
-      <c r="F26" s="68">
+      <c r="F26" s="70">
         <v>-20</v>
       </c>
       <c r="G26" s="45" t="s">
@@ -10661,8 +10706,8 @@
         <v>1000000000</v>
       </c>
       <c r="L26" s="53">
-        <f>(R26+'Frequency Range Setting'!$B$7)*1000000</f>
-        <v>1805000000</v>
+        <f>((R26+'Frequency Range Setting'!$B$7)*1000000)+$U$2</f>
+        <v>1805500000</v>
       </c>
       <c r="M26" s="39">
         <v>150000</v>
@@ -10674,8 +10719,8 @@
         <v>1000000000</v>
       </c>
       <c r="P26" s="53">
-        <f>(R26-'Frequency Range Setting'!$B$7)*1000000</f>
-        <v>1735000000</v>
+        <f>((R26-'Frequency Range Setting'!$B$7)*1000000)-$U$2</f>
+        <v>1734500000</v>
       </c>
       <c r="Q26" s="39">
         <v>12750000000</v>
@@ -10699,7 +10744,7 @@
       <c r="E27" s="44">
         <v>0</v>
       </c>
-      <c r="F27" s="68">
+      <c r="F27" s="70">
         <v>-20</v>
       </c>
       <c r="G27" s="45" t="s">
@@ -10718,8 +10763,8 @@
         <v>1000000000</v>
       </c>
       <c r="L27" s="53">
-        <f>(R27+'Frequency Range Setting'!$B$7)*1000000</f>
-        <v>1805000000</v>
+        <f>((R27+'Frequency Range Setting'!$B$7)*1000000)+$U$2</f>
+        <v>1805500000</v>
       </c>
       <c r="M27" s="39">
         <v>150000</v>
@@ -10731,8 +10776,8 @@
         <v>1000000000</v>
       </c>
       <c r="P27" s="53">
-        <f>(R27-'Frequency Range Setting'!$B$7)*1000000</f>
-        <v>1735000000</v>
+        <f>((R27-'Frequency Range Setting'!$B$7)*1000000)-$U$2</f>
+        <v>1734500000</v>
       </c>
       <c r="Q27" s="39">
         <v>12750000000</v>
@@ -10756,7 +10801,7 @@
       <c r="E28" s="44">
         <v>99</v>
       </c>
-      <c r="F28" s="68">
+      <c r="F28" s="70">
         <v>-20</v>
       </c>
       <c r="G28" s="45" t="s">
@@ -10775,8 +10820,8 @@
         <v>1000000000</v>
       </c>
       <c r="L28" s="53">
-        <f>(R28+'Frequency Range Setting'!$B$7)*1000000</f>
-        <v>1805000000</v>
+        <f>((R28+'Frequency Range Setting'!$B$7)*1000000)+$U$2</f>
+        <v>1805500000</v>
       </c>
       <c r="M28" s="39">
         <v>150000</v>
@@ -10788,8 +10833,8 @@
         <v>1000000000</v>
       </c>
       <c r="P28" s="53">
-        <f>(R28-'Frequency Range Setting'!$B$7)*1000000</f>
-        <v>1735000000</v>
+        <f>((R28-'Frequency Range Setting'!$B$7)*1000000)-$U$2</f>
+        <v>1734500000</v>
       </c>
       <c r="Q28" s="39">
         <v>12750000000</v>
@@ -10821,7 +10866,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
@@ -11203,7 +11248,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -11393,7 +11438,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
@@ -11520,7 +11565,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
@@ -11647,7 +11692,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
@@ -11762,13 +11807,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -11779,7 +11824,7 @@
         <v>3.5</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -11790,7 +11835,7 @@
         <v>5</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -11801,7 +11846,7 @@
         <v>12.5</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -11812,7 +11857,7 @@
         <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -11823,7 +11868,7 @@
         <v>27.5</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -11836,78 +11881,78 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B16" s="30" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s">
         <v>35</v>
       </c>
-      <c r="C19" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" t="s">
-        <v>34</v>
-      </c>
       <c r="E19" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -12014,91 +12059,91 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D27" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C28" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D28" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" s="30" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C29" s="30" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D29" s="30" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C30" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D30" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" s="29" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D31" s="29" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="32" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C33" s="32" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D33" s="32" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E33" s="32"/>
       <c r="F33" s="32"/>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="32" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C34" s="32" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D34" s="32" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E34" s="32"/>
       <c r="F34" s="32"/>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="33" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C35" s="33" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D35" s="35" t="e">
         <f>Band5!#REF!</f>
@@ -12111,7 +12156,7 @@
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="34" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C36" s="36" t="e">
         <f>Band5!#REF!</f>
@@ -12130,14 +12175,14 @@
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="34" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C37" s="36" t="e">
         <f>Band5!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="D37" s="34" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E37" s="32">
         <v>1000</v>

</xml_diff>

<commit_message>
modified:   Band2MaxPowerInput1_FrequencySweepRanges.xlsx 	modified:   Band2MinPowerInput1_FrequencySweepRanges.xlsx
</commit_message>
<xml_diff>
--- a/Band2MinPowerInput1_FrequencySweepRanges.xlsx
+++ b/Band2MinPowerInput1_FrequencySweepRanges.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hclo365-my.sharepoint.com/personal/aayush_jain_hcl_com/Documents/Facebook/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Test\DVT-Wireless-HCL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="412" documentId="13_ncr:1_{29D0E568-EE65-415B-89C9-359224AD92FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{3C376A60-873D-4805-BB3B-0FB2E91BD418}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC55430-1671-48B3-98B4-95F4579CFA8B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{BA741C37-369C-4D69-BC66-4EE94A3A8637}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{BA741C37-369C-4D69-BC66-4EE94A3A8637}"/>
   </bookViews>
   <sheets>
     <sheet name="Band2" sheetId="1" r:id="rId1"/>
@@ -917,7 +917,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F21EF5-0615-4121-83E8-517FC8180B1A}">
   <dimension ref="A1:AK28"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1058,8 +1060,8 @@
       <c r="E2" s="51">
         <v>0</v>
       </c>
-      <c r="F2" s="52">
-        <v>23</v>
+      <c r="F2" s="68">
+        <v>-20</v>
       </c>
       <c r="G2" s="39" t="s">
         <v>7</v>
@@ -1156,8 +1158,8 @@
       <c r="E3" s="51">
         <v>0</v>
       </c>
-      <c r="F3" s="52">
-        <v>23</v>
+      <c r="F3" s="68">
+        <v>-20</v>
       </c>
       <c r="G3" s="39" t="s">
         <v>7</v>
@@ -1255,8 +1257,8 @@
       <c r="E4" s="51">
         <v>5</v>
       </c>
-      <c r="F4" s="52">
-        <v>23</v>
+      <c r="F4" s="68">
+        <v>-20</v>
       </c>
       <c r="G4" s="39" t="s">
         <v>7</v>
@@ -1357,8 +1359,8 @@
       <c r="E5" s="51">
         <v>0</v>
       </c>
-      <c r="F5" s="52">
-        <v>23</v>
+      <c r="F5" s="68">
+        <v>-20</v>
       </c>
       <c r="G5" s="39" t="s">
         <v>7</v>
@@ -1459,8 +1461,8 @@
       <c r="E6" s="51">
         <v>0</v>
       </c>
-      <c r="F6" s="52">
-        <v>23</v>
+      <c r="F6" s="68">
+        <v>-20</v>
       </c>
       <c r="G6" s="39" t="s">
         <v>7</v>
@@ -1549,8 +1551,8 @@
       <c r="E7" s="51">
         <v>24</v>
       </c>
-      <c r="F7" s="52">
-        <v>23</v>
+      <c r="F7" s="68">
+        <v>-20</v>
       </c>
       <c r="G7" s="39" t="s">
         <v>7</v>
@@ -1639,8 +1641,8 @@
       <c r="E8" s="51">
         <v>0</v>
       </c>
-      <c r="F8" s="52">
-        <v>23</v>
+      <c r="F8" s="68">
+        <v>-20</v>
       </c>
       <c r="G8" s="39" t="s">
         <v>7</v>
@@ -1739,8 +1741,8 @@
       <c r="E9" s="51">
         <v>0</v>
       </c>
-      <c r="F9" s="52">
-        <v>23</v>
+      <c r="F9" s="68">
+        <v>-20</v>
       </c>
       <c r="G9" s="39" t="s">
         <v>7</v>
@@ -1832,8 +1834,8 @@
       <c r="E10" s="51">
         <v>99</v>
       </c>
-      <c r="F10" s="52">
-        <v>23</v>
+      <c r="F10" s="68">
+        <v>-20</v>
       </c>
       <c r="G10" s="39" t="s">
         <v>7</v>
@@ -1933,8 +1935,8 @@
       <c r="E11" s="41">
         <v>0</v>
       </c>
-      <c r="F11" s="43">
-        <v>23</v>
+      <c r="F11" s="68">
+        <v>-20</v>
       </c>
       <c r="G11" s="42" t="s">
         <v>8</v>
@@ -2023,8 +2025,8 @@
       <c r="E12" s="41">
         <v>0</v>
       </c>
-      <c r="F12" s="43">
-        <v>23</v>
+      <c r="F12" s="68">
+        <v>-20</v>
       </c>
       <c r="G12" s="42" t="s">
         <v>8</v>
@@ -2113,8 +2115,8 @@
       <c r="E13" s="41">
         <v>5</v>
       </c>
-      <c r="F13" s="43">
-        <v>23</v>
+      <c r="F13" s="68">
+        <v>-20</v>
       </c>
       <c r="G13" s="42" t="s">
         <v>8</v>
@@ -2203,8 +2205,8 @@
       <c r="E14" s="41">
         <v>0</v>
       </c>
-      <c r="F14" s="43">
-        <v>23</v>
+      <c r="F14" s="68">
+        <v>-20</v>
       </c>
       <c r="G14" s="42" t="s">
         <v>8</v>
@@ -2293,8 +2295,8 @@
       <c r="E15" s="41">
         <v>0</v>
       </c>
-      <c r="F15" s="43">
-        <v>23</v>
+      <c r="F15" s="68">
+        <v>-20</v>
       </c>
       <c r="G15" s="42" t="s">
         <v>8</v>
@@ -2386,8 +2388,8 @@
       <c r="E16" s="41">
         <v>24</v>
       </c>
-      <c r="F16" s="43">
-        <v>23</v>
+      <c r="F16" s="68">
+        <v>-20</v>
       </c>
       <c r="G16" s="42" t="s">
         <v>8</v>
@@ -2479,8 +2481,8 @@
       <c r="E17" s="41">
         <v>0</v>
       </c>
-      <c r="F17" s="43">
-        <v>23</v>
+      <c r="F17" s="68">
+        <v>-20</v>
       </c>
       <c r="G17" s="42" t="s">
         <v>8</v>
@@ -2572,8 +2574,8 @@
       <c r="E18" s="41">
         <v>0</v>
       </c>
-      <c r="F18" s="43">
-        <v>23</v>
+      <c r="F18" s="68">
+        <v>-20</v>
       </c>
       <c r="G18" s="42" t="s">
         <v>8</v>
@@ -2665,8 +2667,8 @@
       <c r="E19" s="41">
         <v>99</v>
       </c>
-      <c r="F19" s="43">
-        <v>23</v>
+      <c r="F19" s="68">
+        <v>-20</v>
       </c>
       <c r="G19" s="42" t="s">
         <v>8</v>
@@ -2758,8 +2760,8 @@
       <c r="E20" s="44">
         <v>0</v>
       </c>
-      <c r="F20" s="46">
-        <v>23</v>
+      <c r="F20" s="68">
+        <v>-20</v>
       </c>
       <c r="G20" s="45" t="s">
         <v>9</v>
@@ -2851,8 +2853,8 @@
       <c r="E21" s="44">
         <v>0</v>
       </c>
-      <c r="F21" s="46">
-        <v>23</v>
+      <c r="F21" s="68">
+        <v>-20</v>
       </c>
       <c r="G21" s="45" t="s">
         <v>9</v>
@@ -2944,8 +2946,8 @@
       <c r="E22" s="44">
         <v>5</v>
       </c>
-      <c r="F22" s="46">
-        <v>23</v>
+      <c r="F22" s="68">
+        <v>-20</v>
       </c>
       <c r="G22" s="45" t="s">
         <v>9</v>
@@ -3037,8 +3039,8 @@
       <c r="E23" s="44">
         <v>0</v>
       </c>
-      <c r="F23" s="46">
-        <v>23</v>
+      <c r="F23" s="68">
+        <v>-20</v>
       </c>
       <c r="G23" s="45" t="s">
         <v>9</v>
@@ -3130,8 +3132,8 @@
       <c r="E24" s="44">
         <v>0</v>
       </c>
-      <c r="F24" s="46">
-        <v>23</v>
+      <c r="F24" s="68">
+        <v>-20</v>
       </c>
       <c r="G24" s="45" t="s">
         <v>9</v>
@@ -3223,8 +3225,8 @@
       <c r="E25" s="44">
         <v>24</v>
       </c>
-      <c r="F25" s="46">
-        <v>23</v>
+      <c r="F25" s="68">
+        <v>-20</v>
       </c>
       <c r="G25" s="45" t="s">
         <v>9</v>
@@ -3313,8 +3315,8 @@
       <c r="E26" s="44">
         <v>0</v>
       </c>
-      <c r="F26" s="46">
-        <v>23</v>
+      <c r="F26" s="68">
+        <v>-20</v>
       </c>
       <c r="G26" s="45" t="s">
         <v>9</v>
@@ -3406,8 +3408,8 @@
       <c r="E27" s="44">
         <v>0</v>
       </c>
-      <c r="F27" s="46">
-        <v>23</v>
+      <c r="F27" s="68">
+        <v>-20</v>
       </c>
       <c r="G27" s="45" t="s">
         <v>9</v>
@@ -3499,8 +3501,8 @@
       <c r="E28" s="44">
         <v>99</v>
       </c>
-      <c r="F28" s="46">
-        <v>23</v>
+      <c r="F28" s="68">
+        <v>-20</v>
       </c>
       <c r="G28" s="45" t="s">
         <v>9</v>
@@ -3589,8 +3591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{855F8828-1D8C-4AAA-81FD-7AC3397EB1C9}">
   <dimension ref="A1:U28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3691,8 +3693,8 @@
       <c r="E2" s="51">
         <v>0</v>
       </c>
-      <c r="F2" s="52">
-        <v>23</v>
+      <c r="F2" s="68">
+        <v>-20</v>
       </c>
       <c r="G2" s="39" t="s">
         <v>7</v>
@@ -3755,8 +3757,8 @@
       <c r="E3" s="51">
         <v>0</v>
       </c>
-      <c r="F3" s="52">
-        <v>23</v>
+      <c r="F3" s="68">
+        <v>-20</v>
       </c>
       <c r="G3" s="39" t="s">
         <v>7</v>
@@ -3812,8 +3814,8 @@
       <c r="E4" s="51">
         <v>5</v>
       </c>
-      <c r="F4" s="52">
-        <v>23</v>
+      <c r="F4" s="68">
+        <v>-20</v>
       </c>
       <c r="G4" s="39" t="s">
         <v>7</v>
@@ -3869,8 +3871,8 @@
       <c r="E5" s="51">
         <v>0</v>
       </c>
-      <c r="F5" s="52">
-        <v>23</v>
+      <c r="F5" s="68">
+        <v>-20</v>
       </c>
       <c r="G5" s="39" t="s">
         <v>7</v>
@@ -3926,8 +3928,8 @@
       <c r="E6" s="51">
         <v>0</v>
       </c>
-      <c r="F6" s="52">
-        <v>23</v>
+      <c r="F6" s="68">
+        <v>-20</v>
       </c>
       <c r="G6" s="39" t="s">
         <v>7</v>
@@ -3983,8 +3985,8 @@
       <c r="E7" s="51">
         <v>24</v>
       </c>
-      <c r="F7" s="52">
-        <v>23</v>
+      <c r="F7" s="68">
+        <v>-20</v>
       </c>
       <c r="G7" s="39" t="s">
         <v>7</v>
@@ -4040,8 +4042,8 @@
       <c r="E8" s="51">
         <v>0</v>
       </c>
-      <c r="F8" s="52">
-        <v>23</v>
+      <c r="F8" s="68">
+        <v>-20</v>
       </c>
       <c r="G8" s="39" t="s">
         <v>7</v>
@@ -4097,8 +4099,8 @@
       <c r="E9" s="51">
         <v>0</v>
       </c>
-      <c r="F9" s="52">
-        <v>23</v>
+      <c r="F9" s="68">
+        <v>-20</v>
       </c>
       <c r="G9" s="39" t="s">
         <v>7</v>
@@ -4154,8 +4156,8 @@
       <c r="E10" s="51">
         <v>99</v>
       </c>
-      <c r="F10" s="52">
-        <v>23</v>
+      <c r="F10" s="68">
+        <v>-20</v>
       </c>
       <c r="G10" s="39" t="s">
         <v>7</v>
@@ -4211,8 +4213,8 @@
       <c r="E11" s="41">
         <v>0</v>
       </c>
-      <c r="F11" s="43">
-        <v>23</v>
+      <c r="F11" s="68">
+        <v>-20</v>
       </c>
       <c r="G11" s="42" t="s">
         <v>8</v>
@@ -4268,8 +4270,8 @@
       <c r="E12" s="41">
         <v>0</v>
       </c>
-      <c r="F12" s="43">
-        <v>23</v>
+      <c r="F12" s="68">
+        <v>-20</v>
       </c>
       <c r="G12" s="42" t="s">
         <v>8</v>
@@ -4325,8 +4327,8 @@
       <c r="E13" s="41">
         <v>5</v>
       </c>
-      <c r="F13" s="43">
-        <v>23</v>
+      <c r="F13" s="68">
+        <v>-20</v>
       </c>
       <c r="G13" s="42" t="s">
         <v>8</v>
@@ -4382,8 +4384,8 @@
       <c r="E14" s="41">
         <v>0</v>
       </c>
-      <c r="F14" s="43">
-        <v>23</v>
+      <c r="F14" s="68">
+        <v>-20</v>
       </c>
       <c r="G14" s="42" t="s">
         <v>8</v>
@@ -4439,8 +4441,8 @@
       <c r="E15" s="41">
         <v>0</v>
       </c>
-      <c r="F15" s="43">
-        <v>23</v>
+      <c r="F15" s="68">
+        <v>-20</v>
       </c>
       <c r="G15" s="42" t="s">
         <v>8</v>
@@ -4496,8 +4498,8 @@
       <c r="E16" s="41">
         <v>24</v>
       </c>
-      <c r="F16" s="43">
-        <v>23</v>
+      <c r="F16" s="68">
+        <v>-20</v>
       </c>
       <c r="G16" s="42" t="s">
         <v>8</v>
@@ -4553,8 +4555,8 @@
       <c r="E17" s="41">
         <v>0</v>
       </c>
-      <c r="F17" s="43">
-        <v>23</v>
+      <c r="F17" s="68">
+        <v>-20</v>
       </c>
       <c r="G17" s="42" t="s">
         <v>8</v>
@@ -4610,8 +4612,8 @@
       <c r="E18" s="41">
         <v>0</v>
       </c>
-      <c r="F18" s="43">
-        <v>23</v>
+      <c r="F18" s="68">
+        <v>-20</v>
       </c>
       <c r="G18" s="42" t="s">
         <v>8</v>
@@ -4667,8 +4669,8 @@
       <c r="E19" s="41">
         <v>99</v>
       </c>
-      <c r="F19" s="43">
-        <v>23</v>
+      <c r="F19" s="68">
+        <v>-20</v>
       </c>
       <c r="G19" s="42" t="s">
         <v>8</v>
@@ -4724,8 +4726,8 @@
       <c r="E20" s="44">
         <v>0</v>
       </c>
-      <c r="F20" s="46">
-        <v>23</v>
+      <c r="F20" s="68">
+        <v>-20</v>
       </c>
       <c r="G20" s="45" t="s">
         <v>9</v>
@@ -4781,8 +4783,8 @@
       <c r="E21" s="44">
         <v>0</v>
       </c>
-      <c r="F21" s="46">
-        <v>23</v>
+      <c r="F21" s="68">
+        <v>-20</v>
       </c>
       <c r="G21" s="45" t="s">
         <v>9</v>
@@ -4838,8 +4840,8 @@
       <c r="E22" s="44">
         <v>5</v>
       </c>
-      <c r="F22" s="46">
-        <v>23</v>
+      <c r="F22" s="68">
+        <v>-20</v>
       </c>
       <c r="G22" s="45" t="s">
         <v>9</v>
@@ -4895,8 +4897,8 @@
       <c r="E23" s="44">
         <v>0</v>
       </c>
-      <c r="F23" s="46">
-        <v>23</v>
+      <c r="F23" s="68">
+        <v>-20</v>
       </c>
       <c r="G23" s="45" t="s">
         <v>9</v>
@@ -4952,8 +4954,8 @@
       <c r="E24" s="44">
         <v>0</v>
       </c>
-      <c r="F24" s="46">
-        <v>23</v>
+      <c r="F24" s="68">
+        <v>-20</v>
       </c>
       <c r="G24" s="45" t="s">
         <v>9</v>
@@ -5009,8 +5011,8 @@
       <c r="E25" s="44">
         <v>24</v>
       </c>
-      <c r="F25" s="46">
-        <v>23</v>
+      <c r="F25" s="68">
+        <v>-20</v>
       </c>
       <c r="G25" s="45" t="s">
         <v>9</v>
@@ -5066,8 +5068,8 @@
       <c r="E26" s="44">
         <v>0</v>
       </c>
-      <c r="F26" s="46">
-        <v>23</v>
+      <c r="F26" s="68">
+        <v>-20</v>
       </c>
       <c r="G26" s="45" t="s">
         <v>9</v>
@@ -5123,8 +5125,8 @@
       <c r="E27" s="44">
         <v>0</v>
       </c>
-      <c r="F27" s="46">
-        <v>23</v>
+      <c r="F27" s="68">
+        <v>-20</v>
       </c>
       <c r="G27" s="45" t="s">
         <v>9</v>
@@ -5180,8 +5182,8 @@
       <c r="E28" s="44">
         <v>99</v>
       </c>
-      <c r="F28" s="46">
-        <v>23</v>
+      <c r="F28" s="68">
+        <v>-20</v>
       </c>
       <c r="G28" s="45" t="s">
         <v>9</v>
@@ -5232,8 +5234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8596D56-7C71-4D72-A666-9CAEA981CBE7}">
   <dimension ref="A1:U60"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5335,8 +5337,8 @@
       <c r="E2" s="64">
         <v>0</v>
       </c>
-      <c r="F2" s="65">
-        <v>23</v>
+      <c r="F2" s="68">
+        <v>-20</v>
       </c>
       <c r="G2" s="54" t="s">
         <v>7</v>
@@ -5399,8 +5401,8 @@
       <c r="E3" s="64">
         <v>0</v>
       </c>
-      <c r="F3" s="65">
-        <v>23</v>
+      <c r="F3" s="68">
+        <v>-20</v>
       </c>
       <c r="G3" s="54" t="s">
         <v>7</v>
@@ -5456,8 +5458,8 @@
       <c r="E4" s="64">
         <v>5</v>
       </c>
-      <c r="F4" s="65">
-        <v>23</v>
+      <c r="F4" s="68">
+        <v>-20</v>
       </c>
       <c r="G4" s="54" t="s">
         <v>7</v>
@@ -5513,8 +5515,8 @@
       <c r="E5" s="64">
         <v>0</v>
       </c>
-      <c r="F5" s="65">
-        <v>23</v>
+      <c r="F5" s="68">
+        <v>-20</v>
       </c>
       <c r="G5" s="54" t="s">
         <v>7</v>
@@ -5570,8 +5572,8 @@
       <c r="E6" s="64">
         <v>0</v>
       </c>
-      <c r="F6" s="65">
-        <v>23</v>
+      <c r="F6" s="68">
+        <v>-20</v>
       </c>
       <c r="G6" s="54" t="s">
         <v>7</v>
@@ -5627,8 +5629,8 @@
       <c r="E7" s="64">
         <v>24</v>
       </c>
-      <c r="F7" s="65">
-        <v>23</v>
+      <c r="F7" s="68">
+        <v>-20</v>
       </c>
       <c r="G7" s="54" t="s">
         <v>7</v>
@@ -5684,8 +5686,8 @@
       <c r="E8" s="64">
         <v>0</v>
       </c>
-      <c r="F8" s="65">
-        <v>23</v>
+      <c r="F8" s="68">
+        <v>-20</v>
       </c>
       <c r="G8" s="54" t="s">
         <v>7</v>
@@ -5741,8 +5743,8 @@
       <c r="E9" s="64">
         <v>0</v>
       </c>
-      <c r="F9" s="65">
-        <v>23</v>
+      <c r="F9" s="68">
+        <v>-20</v>
       </c>
       <c r="G9" s="54" t="s">
         <v>7</v>
@@ -5798,8 +5800,8 @@
       <c r="E10" s="64">
         <v>49</v>
       </c>
-      <c r="F10" s="65">
-        <v>23</v>
+      <c r="F10" s="68">
+        <v>-20</v>
       </c>
       <c r="G10" s="54" t="s">
         <v>7</v>
@@ -5855,8 +5857,8 @@
       <c r="E11" s="64">
         <v>0</v>
       </c>
-      <c r="F11" s="65">
-        <v>23</v>
+      <c r="F11" s="68">
+        <v>-20</v>
       </c>
       <c r="G11" s="54" t="s">
         <v>8</v>
@@ -5912,8 +5914,8 @@
       <c r="E12" s="64">
         <v>0</v>
       </c>
-      <c r="F12" s="65">
-        <v>23</v>
+      <c r="F12" s="68">
+        <v>-20</v>
       </c>
       <c r="G12" s="54" t="s">
         <v>8</v>
@@ -5969,8 +5971,8 @@
       <c r="E13" s="64">
         <v>5</v>
       </c>
-      <c r="F13" s="65">
-        <v>23</v>
+      <c r="F13" s="68">
+        <v>-20</v>
       </c>
       <c r="G13" s="54" t="s">
         <v>8</v>
@@ -6026,8 +6028,8 @@
       <c r="E14" s="64">
         <v>0</v>
       </c>
-      <c r="F14" s="65">
-        <v>23</v>
+      <c r="F14" s="68">
+        <v>-20</v>
       </c>
       <c r="G14" s="54" t="s">
         <v>8</v>
@@ -6083,8 +6085,8 @@
       <c r="E15" s="64">
         <v>0</v>
       </c>
-      <c r="F15" s="65">
-        <v>23</v>
+      <c r="F15" s="68">
+        <v>-20</v>
       </c>
       <c r="G15" s="54" t="s">
         <v>8</v>
@@ -6140,8 +6142,8 @@
       <c r="E16" s="64">
         <v>24</v>
       </c>
-      <c r="F16" s="65">
-        <v>23</v>
+      <c r="F16" s="68">
+        <v>-20</v>
       </c>
       <c r="G16" s="54" t="s">
         <v>8</v>
@@ -6197,8 +6199,8 @@
       <c r="E17" s="64">
         <v>0</v>
       </c>
-      <c r="F17" s="65">
-        <v>23</v>
+      <c r="F17" s="68">
+        <v>-20</v>
       </c>
       <c r="G17" s="54" t="s">
         <v>8</v>
@@ -6254,8 +6256,8 @@
       <c r="E18" s="64">
         <v>0</v>
       </c>
-      <c r="F18" s="65">
-        <v>23</v>
+      <c r="F18" s="68">
+        <v>-20</v>
       </c>
       <c r="G18" s="54" t="s">
         <v>8</v>
@@ -6311,8 +6313,8 @@
       <c r="E19" s="64">
         <v>49</v>
       </c>
-      <c r="F19" s="65">
-        <v>23</v>
+      <c r="F19" s="68">
+        <v>-20</v>
       </c>
       <c r="G19" s="54" t="s">
         <v>8</v>
@@ -6368,8 +6370,8 @@
       <c r="E20" s="64">
         <v>0</v>
       </c>
-      <c r="F20" s="65">
-        <v>23</v>
+      <c r="F20" s="68">
+        <v>-20</v>
       </c>
       <c r="G20" s="54" t="s">
         <v>9</v>
@@ -6425,8 +6427,8 @@
       <c r="E21" s="64">
         <v>0</v>
       </c>
-      <c r="F21" s="65">
-        <v>23</v>
+      <c r="F21" s="68">
+        <v>-20</v>
       </c>
       <c r="G21" s="54" t="s">
         <v>9</v>
@@ -6482,8 +6484,8 @@
       <c r="E22" s="64">
         <v>5</v>
       </c>
-      <c r="F22" s="65">
-        <v>23</v>
+      <c r="F22" s="68">
+        <v>-20</v>
       </c>
       <c r="G22" s="54" t="s">
         <v>9</v>
@@ -6539,8 +6541,8 @@
       <c r="E23" s="64">
         <v>0</v>
       </c>
-      <c r="F23" s="65">
-        <v>23</v>
+      <c r="F23" s="68">
+        <v>-20</v>
       </c>
       <c r="G23" s="54" t="s">
         <v>9</v>
@@ -6596,8 +6598,8 @@
       <c r="E24" s="64">
         <v>0</v>
       </c>
-      <c r="F24" s="65">
-        <v>23</v>
+      <c r="F24" s="68">
+        <v>-20</v>
       </c>
       <c r="G24" s="54" t="s">
         <v>9</v>
@@ -6653,8 +6655,8 @@
       <c r="E25" s="64">
         <v>24</v>
       </c>
-      <c r="F25" s="65">
-        <v>23</v>
+      <c r="F25" s="68">
+        <v>-20</v>
       </c>
       <c r="G25" s="54" t="s">
         <v>9</v>
@@ -6710,8 +6712,8 @@
       <c r="E26" s="64">
         <v>0</v>
       </c>
-      <c r="F26" s="65">
-        <v>23</v>
+      <c r="F26" s="68">
+        <v>-20</v>
       </c>
       <c r="G26" s="54" t="s">
         <v>9</v>
@@ -6767,8 +6769,8 @@
       <c r="E27" s="64">
         <v>0</v>
       </c>
-      <c r="F27" s="65">
-        <v>23</v>
+      <c r="F27" s="68">
+        <v>-20</v>
       </c>
       <c r="G27" s="54" t="s">
         <v>9</v>
@@ -6824,8 +6826,8 @@
       <c r="E28" s="64">
         <v>49</v>
       </c>
-      <c r="F28" s="65">
-        <v>23</v>
+      <c r="F28" s="68">
+        <v>-20</v>
       </c>
       <c r="G28" s="54" t="s">
         <v>9</v>
@@ -6901,8 +6903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D108741B-A8D0-4BB3-B12C-6B68B68001DF}">
   <dimension ref="A1:U28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7004,8 +7006,8 @@
       <c r="E2" s="51">
         <v>0</v>
       </c>
-      <c r="F2" s="52">
-        <v>23</v>
+      <c r="F2" s="68">
+        <v>-20</v>
       </c>
       <c r="G2" s="39" t="s">
         <v>7</v>
@@ -7068,8 +7070,8 @@
       <c r="E3" s="51">
         <v>0</v>
       </c>
-      <c r="F3" s="52">
-        <v>23</v>
+      <c r="F3" s="68">
+        <v>-20</v>
       </c>
       <c r="G3" s="39" t="s">
         <v>7</v>
@@ -7125,8 +7127,8 @@
       <c r="E4" s="51">
         <v>5</v>
       </c>
-      <c r="F4" s="52">
-        <v>23</v>
+      <c r="F4" s="68">
+        <v>-20</v>
       </c>
       <c r="G4" s="39" t="s">
         <v>7</v>
@@ -7182,8 +7184,8 @@
       <c r="E5" s="51">
         <v>0</v>
       </c>
-      <c r="F5" s="52">
-        <v>23</v>
+      <c r="F5" s="68">
+        <v>-20</v>
       </c>
       <c r="G5" s="39" t="s">
         <v>7</v>
@@ -7239,8 +7241,8 @@
       <c r="E6" s="51">
         <v>0</v>
       </c>
-      <c r="F6" s="52">
-        <v>23</v>
+      <c r="F6" s="68">
+        <v>-20</v>
       </c>
       <c r="G6" s="39" t="s">
         <v>7</v>
@@ -7296,8 +7298,8 @@
       <c r="E7" s="51">
         <v>24</v>
       </c>
-      <c r="F7" s="52">
-        <v>23</v>
+      <c r="F7" s="68">
+        <v>-20</v>
       </c>
       <c r="G7" s="39" t="s">
         <v>7</v>
@@ -7353,8 +7355,8 @@
       <c r="E8" s="51">
         <v>0</v>
       </c>
-      <c r="F8" s="52">
-        <v>23</v>
+      <c r="F8" s="68">
+        <v>-20</v>
       </c>
       <c r="G8" s="39" t="s">
         <v>7</v>
@@ -7410,8 +7412,8 @@
       <c r="E9" s="51">
         <v>0</v>
       </c>
-      <c r="F9" s="52">
-        <v>23</v>
+      <c r="F9" s="68">
+        <v>-20</v>
       </c>
       <c r="G9" s="39" t="s">
         <v>7</v>
@@ -7467,8 +7469,8 @@
       <c r="E10" s="51">
         <v>49</v>
       </c>
-      <c r="F10" s="52">
-        <v>23</v>
+      <c r="F10" s="68">
+        <v>-20</v>
       </c>
       <c r="G10" s="39" t="s">
         <v>7</v>
@@ -7524,8 +7526,8 @@
       <c r="E11" s="41">
         <v>0</v>
       </c>
-      <c r="F11" s="43">
-        <v>23</v>
+      <c r="F11" s="68">
+        <v>-20</v>
       </c>
       <c r="G11" s="42" t="s">
         <v>8</v>
@@ -7581,8 +7583,8 @@
       <c r="E12" s="41">
         <v>0</v>
       </c>
-      <c r="F12" s="43">
-        <v>23</v>
+      <c r="F12" s="68">
+        <v>-20</v>
       </c>
       <c r="G12" s="42" t="s">
         <v>8</v>
@@ -7638,8 +7640,8 @@
       <c r="E13" s="41">
         <v>5</v>
       </c>
-      <c r="F13" s="43">
-        <v>23</v>
+      <c r="F13" s="68">
+        <v>-20</v>
       </c>
       <c r="G13" s="42" t="s">
         <v>8</v>
@@ -7695,8 +7697,8 @@
       <c r="E14" s="41">
         <v>0</v>
       </c>
-      <c r="F14" s="43">
-        <v>23</v>
+      <c r="F14" s="68">
+        <v>-20</v>
       </c>
       <c r="G14" s="42" t="s">
         <v>8</v>
@@ -7752,8 +7754,8 @@
       <c r="E15" s="41">
         <v>0</v>
       </c>
-      <c r="F15" s="43">
-        <v>23</v>
+      <c r="F15" s="68">
+        <v>-20</v>
       </c>
       <c r="G15" s="42" t="s">
         <v>8</v>
@@ -7809,8 +7811,8 @@
       <c r="E16" s="41">
         <v>24</v>
       </c>
-      <c r="F16" s="43">
-        <v>23</v>
+      <c r="F16" s="68">
+        <v>-20</v>
       </c>
       <c r="G16" s="42" t="s">
         <v>8</v>
@@ -7866,8 +7868,8 @@
       <c r="E17" s="41">
         <v>0</v>
       </c>
-      <c r="F17" s="43">
-        <v>23</v>
+      <c r="F17" s="68">
+        <v>-20</v>
       </c>
       <c r="G17" s="42" t="s">
         <v>8</v>
@@ -7923,8 +7925,8 @@
       <c r="E18" s="41">
         <v>0</v>
       </c>
-      <c r="F18" s="43">
-        <v>23</v>
+      <c r="F18" s="68">
+        <v>-20</v>
       </c>
       <c r="G18" s="42" t="s">
         <v>8</v>
@@ -7980,8 +7982,8 @@
       <c r="E19" s="41">
         <v>49</v>
       </c>
-      <c r="F19" s="43">
-        <v>23</v>
+      <c r="F19" s="68">
+        <v>-20</v>
       </c>
       <c r="G19" s="42" t="s">
         <v>8</v>
@@ -8037,8 +8039,8 @@
       <c r="E20" s="44">
         <v>0</v>
       </c>
-      <c r="F20" s="46">
-        <v>23</v>
+      <c r="F20" s="68">
+        <v>-20</v>
       </c>
       <c r="G20" s="45" t="s">
         <v>9</v>
@@ -8094,8 +8096,8 @@
       <c r="E21" s="44">
         <v>0</v>
       </c>
-      <c r="F21" s="46">
-        <v>23</v>
+      <c r="F21" s="68">
+        <v>-20</v>
       </c>
       <c r="G21" s="45" t="s">
         <v>9</v>
@@ -8151,8 +8153,8 @@
       <c r="E22" s="44">
         <v>5</v>
       </c>
-      <c r="F22" s="46">
-        <v>23</v>
+      <c r="F22" s="68">
+        <v>-20</v>
       </c>
       <c r="G22" s="45" t="s">
         <v>9</v>
@@ -8208,8 +8210,8 @@
       <c r="E23" s="44">
         <v>0</v>
       </c>
-      <c r="F23" s="46">
-        <v>23</v>
+      <c r="F23" s="68">
+        <v>-20</v>
       </c>
       <c r="G23" s="45" t="s">
         <v>9</v>
@@ -8265,8 +8267,8 @@
       <c r="E24" s="44">
         <v>0</v>
       </c>
-      <c r="F24" s="46">
-        <v>23</v>
+      <c r="F24" s="68">
+        <v>-20</v>
       </c>
       <c r="G24" s="45" t="s">
         <v>9</v>
@@ -8322,8 +8324,8 @@
       <c r="E25" s="44">
         <v>24</v>
       </c>
-      <c r="F25" s="46">
-        <v>23</v>
+      <c r="F25" s="68">
+        <v>-20</v>
       </c>
       <c r="G25" s="45" t="s">
         <v>9</v>
@@ -8379,8 +8381,8 @@
       <c r="E26" s="44">
         <v>0</v>
       </c>
-      <c r="F26" s="46">
-        <v>23</v>
+      <c r="F26" s="68">
+        <v>-20</v>
       </c>
       <c r="G26" s="45" t="s">
         <v>9</v>
@@ -8436,8 +8438,8 @@
       <c r="E27" s="44">
         <v>0</v>
       </c>
-      <c r="F27" s="46">
-        <v>23</v>
+      <c r="F27" s="68">
+        <v>-20</v>
       </c>
       <c r="G27" s="45" t="s">
         <v>9</v>
@@ -8493,8 +8495,8 @@
       <c r="E28" s="44">
         <v>49</v>
       </c>
-      <c r="F28" s="46">
-        <v>23</v>
+      <c r="F28" s="68">
+        <v>-20</v>
       </c>
       <c r="G28" s="45" t="s">
         <v>9</v>
@@ -8543,10 +8545,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDABD784-AD31-46F2-99DC-A4DD1B41AE1B}">
-  <dimension ref="A1:U13"/>
+  <dimension ref="A1:U28"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14:F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8647,8 +8649,8 @@
       <c r="E2" s="51">
         <v>0</v>
       </c>
-      <c r="F2" s="52">
-        <v>23</v>
+      <c r="F2" s="68">
+        <v>-20</v>
       </c>
       <c r="G2" s="39" t="s">
         <v>7</v>
@@ -8711,8 +8713,8 @@
       <c r="E3" s="51">
         <v>0</v>
       </c>
-      <c r="F3" s="52">
-        <v>23</v>
+      <c r="F3" s="68">
+        <v>-20</v>
       </c>
       <c r="G3" s="39" t="s">
         <v>7</v>
@@ -8768,8 +8770,8 @@
       <c r="E4" s="51">
         <v>24</v>
       </c>
-      <c r="F4" s="52">
-        <v>23</v>
+      <c r="F4" s="68">
+        <v>-20</v>
       </c>
       <c r="G4" s="39" t="s">
         <v>7</v>
@@ -8825,8 +8827,8 @@
       <c r="E5" s="51">
         <v>0</v>
       </c>
-      <c r="F5" s="52">
-        <v>23</v>
+      <c r="F5" s="68">
+        <v>-20</v>
       </c>
       <c r="G5" s="39" t="s">
         <v>8</v>
@@ -8882,8 +8884,8 @@
       <c r="E6" s="51">
         <v>0</v>
       </c>
-      <c r="F6" s="52">
-        <v>23</v>
+      <c r="F6" s="68">
+        <v>-20</v>
       </c>
       <c r="G6" s="39" t="s">
         <v>8</v>
@@ -8939,8 +8941,8 @@
       <c r="E7" s="51">
         <v>24</v>
       </c>
-      <c r="F7" s="52">
-        <v>23</v>
+      <c r="F7" s="68">
+        <v>-20</v>
       </c>
       <c r="G7" s="39" t="s">
         <v>8</v>
@@ -8996,8 +8998,8 @@
       <c r="E8" s="51">
         <v>0</v>
       </c>
-      <c r="F8" s="52">
-        <v>23</v>
+      <c r="F8" s="68">
+        <v>-20</v>
       </c>
       <c r="G8" s="39" t="s">
         <v>9</v>
@@ -9053,8 +9055,8 @@
       <c r="E9" s="51">
         <v>0</v>
       </c>
-      <c r="F9" s="52">
-        <v>23</v>
+      <c r="F9" s="68">
+        <v>-20</v>
       </c>
       <c r="G9" s="39" t="s">
         <v>9</v>
@@ -9110,8 +9112,8 @@
       <c r="E10" s="51">
         <v>24</v>
       </c>
-      <c r="F10" s="52">
-        <v>23</v>
+      <c r="F10" s="68">
+        <v>-20</v>
       </c>
       <c r="G10" s="39" t="s">
         <v>9</v>
@@ -9167,8 +9169,8 @@
       <c r="E11" s="41">
         <v>0</v>
       </c>
-      <c r="F11" s="52">
-        <v>23</v>
+      <c r="F11" s="68">
+        <v>-20</v>
       </c>
       <c r="G11" s="42" t="s">
         <v>8</v>
@@ -9224,8 +9226,8 @@
       <c r="E12" s="41">
         <v>0</v>
       </c>
-      <c r="F12" s="52">
-        <v>23</v>
+      <c r="F12" s="68">
+        <v>-20</v>
       </c>
       <c r="G12" s="42" t="s">
         <v>8</v>
@@ -9281,8 +9283,8 @@
       <c r="E13" s="41">
         <v>49</v>
       </c>
-      <c r="F13" s="52">
-        <v>23</v>
+      <c r="F13" s="68">
+        <v>-20</v>
       </c>
       <c r="G13" s="42" t="s">
         <v>8</v>
@@ -9323,6 +9325,51 @@
         <f t="shared" si="0"/>
         <v>782</v>
       </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F14" s="68"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F15" s="68"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F16" s="68"/>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="68"/>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="68"/>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="68"/>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F20" s="68"/>
+    </row>
+    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F21" s="68"/>
+    </row>
+    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F22" s="68"/>
+    </row>
+    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F23" s="68"/>
+    </row>
+    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F24" s="68"/>
+    </row>
+    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F25" s="68"/>
+    </row>
+    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F26" s="68"/>
+    </row>
+    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F27" s="68"/>
+    </row>
+    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F28" s="68"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -9334,8 +9381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F7206B6-36E5-4637-B4E1-0FEA65E91330}">
   <dimension ref="A1:U28"/>
   <sheetViews>
-    <sheetView topLeftCell="H8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
modified:   Band2MinPowerInput1_FrequencySweepRanges.xlsx 	modified:   Milan_SW_Upgrade.py
</commit_message>
<xml_diff>
--- a/Band2MinPowerInput1_FrequencySweepRanges.xlsx
+++ b/Band2MinPowerInput1_FrequencySweepRanges.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Test\DVT-Wireless-HCL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC55430-1671-48B3-98B4-95F4579CFA8B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5114547-CBBD-42D8-82ED-74AFD073BD7C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{BA741C37-369C-4D69-BC66-4EE94A3A8637}"/>
+    <workbookView xWindow="2580" yWindow="600" windowWidth="25500" windowHeight="14265" activeTab="1" xr2:uid="{BA741C37-369C-4D69-BC66-4EE94A3A8637}"/>
   </bookViews>
   <sheets>
     <sheet name="Band2" sheetId="1" r:id="rId1"/>
@@ -3591,8 +3591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{855F8828-1D8C-4AAA-81FD-7AC3397EB1C9}">
   <dimension ref="A1:U28"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F28"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4029,24 +4029,24 @@
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="51"/>
-      <c r="B8" s="39">
-        <v>20</v>
-      </c>
-      <c r="C8" s="52">
-        <v>2120</v>
-      </c>
-      <c r="D8" s="51">
-        <v>100</v>
-      </c>
-      <c r="E8" s="51">
+      <c r="A8" s="41"/>
+      <c r="B8" s="42">
+        <v>1.4</v>
+      </c>
+      <c r="C8" s="43">
+        <v>2132.5</v>
+      </c>
+      <c r="D8" s="41">
+        <v>6</v>
+      </c>
+      <c r="E8" s="41">
         <v>0</v>
       </c>
       <c r="F8" s="68">
         <v>-20</v>
       </c>
-      <c r="G8" s="39" t="s">
-        <v>7</v>
+      <c r="G8" s="42" t="s">
+        <v>8</v>
       </c>
       <c r="H8" s="39">
         <v>9000</v>
@@ -4061,8 +4061,8 @@
         <v>1000000000</v>
       </c>
       <c r="L8" s="56">
-        <f>((R8+'Frequency Range Setting'!$B$7)*1000000)+$U$2</f>
-        <v>1755500000</v>
+        <f>((R8+'Frequency Range Setting'!$B$2)*1000000)+$U$2</f>
+        <v>1736500000</v>
       </c>
       <c r="M8" s="39">
         <v>150000</v>
@@ -4074,36 +4074,36 @@
         <v>1000000000</v>
       </c>
       <c r="P8" s="53">
-        <f>((R8-'Frequency Range Setting'!$B$7)*1000000)-$U$2</f>
-        <v>1684500000</v>
+        <f>((R8-'Frequency Range Setting'!$B$2)*1000000)-$U$2</f>
+        <v>1728500000</v>
       </c>
       <c r="Q8" s="39">
         <v>12750000000</v>
       </c>
       <c r="R8" s="57">
         <f t="shared" si="0"/>
-        <v>1720</v>
+        <v>1732.5</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="51"/>
-      <c r="B9" s="39">
-        <v>20</v>
-      </c>
-      <c r="C9" s="52">
-        <v>2120</v>
-      </c>
-      <c r="D9" s="51">
-        <v>1</v>
-      </c>
-      <c r="E9" s="51">
+      <c r="A9" s="41"/>
+      <c r="B9" s="42">
+        <v>1.4</v>
+      </c>
+      <c r="C9" s="43">
+        <v>2132.5</v>
+      </c>
+      <c r="D9" s="41">
+        <v>1</v>
+      </c>
+      <c r="E9" s="41">
         <v>0</v>
       </c>
       <c r="F9" s="68">
         <v>-20</v>
       </c>
-      <c r="G9" s="39" t="s">
-        <v>7</v>
+      <c r="G9" s="42" t="s">
+        <v>8</v>
       </c>
       <c r="H9" s="39">
         <v>9000</v>
@@ -4118,8 +4118,8 @@
         <v>1000000000</v>
       </c>
       <c r="L9" s="56">
-        <f>((R9+'Frequency Range Setting'!$B$7)*1000000)+$U$2</f>
-        <v>1755500000</v>
+        <f>((R9+'Frequency Range Setting'!$B$2)*1000000)+$U$2</f>
+        <v>1736500000</v>
       </c>
       <c r="M9" s="39">
         <v>150000</v>
@@ -4131,36 +4131,36 @@
         <v>1000000000</v>
       </c>
       <c r="P9" s="53">
-        <f>((R9-'Frequency Range Setting'!$B$7)*1000000)-$U$2</f>
-        <v>1684500000</v>
+        <f>((R9-'Frequency Range Setting'!$B$2)*1000000)-$U$2</f>
+        <v>1728500000</v>
       </c>
       <c r="Q9" s="39">
         <v>12750000000</v>
       </c>
       <c r="R9" s="57">
         <f t="shared" si="0"/>
-        <v>1720</v>
+        <v>1732.5</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="51"/>
-      <c r="B10" s="39">
-        <v>20</v>
-      </c>
-      <c r="C10" s="52">
-        <v>2120</v>
-      </c>
-      <c r="D10" s="51">
-        <v>1</v>
-      </c>
-      <c r="E10" s="51">
-        <v>99</v>
+      <c r="A10" s="41"/>
+      <c r="B10" s="42">
+        <v>1.4</v>
+      </c>
+      <c r="C10" s="43">
+        <v>2132.5</v>
+      </c>
+      <c r="D10" s="41">
+        <v>1</v>
+      </c>
+      <c r="E10" s="41">
+        <v>5</v>
       </c>
       <c r="F10" s="68">
         <v>-20</v>
       </c>
-      <c r="G10" s="39" t="s">
-        <v>7</v>
+      <c r="G10" s="42" t="s">
+        <v>8</v>
       </c>
       <c r="H10" s="39">
         <v>9000</v>
@@ -4175,8 +4175,8 @@
         <v>1000000000</v>
       </c>
       <c r="L10" s="56">
-        <f>((R10+'Frequency Range Setting'!$B$7)*1000000)+$U$2</f>
-        <v>1755500000</v>
+        <f>((R10+'Frequency Range Setting'!$B$2)*1000000)+$U$2</f>
+        <v>1736500000</v>
       </c>
       <c r="M10" s="39">
         <v>150000</v>
@@ -4188,27 +4188,27 @@
         <v>1000000000</v>
       </c>
       <c r="P10" s="53">
-        <f>((R10-'Frequency Range Setting'!$B$7)*1000000)-$U$2</f>
-        <v>1684500000</v>
+        <f>((R10-'Frequency Range Setting'!$B$2)*1000000)-$U$2</f>
+        <v>1728500000</v>
       </c>
       <c r="Q10" s="39">
         <v>12750000000</v>
       </c>
       <c r="R10" s="57">
         <f t="shared" si="0"/>
-        <v>1720</v>
+        <v>1732.5</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="41"/>
       <c r="B11" s="42">
-        <v>1.4</v>
+        <v>5</v>
       </c>
       <c r="C11" s="43">
         <v>2132.5</v>
       </c>
       <c r="D11" s="41">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E11" s="41">
         <v>0</v>
@@ -4232,8 +4232,8 @@
         <v>1000000000</v>
       </c>
       <c r="L11" s="56">
-        <f>((R11+'Frequency Range Setting'!$B$2)*1000000)+$U$2</f>
-        <v>1736500000</v>
+        <f>((R11+'Frequency Range Setting'!$B$4)*1000000)+$U$2</f>
+        <v>1745500000</v>
       </c>
       <c r="M11" s="39">
         <v>150000</v>
@@ -4245,8 +4245,8 @@
         <v>1000000000</v>
       </c>
       <c r="P11" s="53">
-        <f>((R11-'Frequency Range Setting'!$B$2)*1000000)-$U$2</f>
-        <v>1728500000</v>
+        <f>((R11-'Frequency Range Setting'!$B$4)*1000000)-$U$2</f>
+        <v>1719500000</v>
       </c>
       <c r="Q11" s="39">
         <v>12750000000</v>
@@ -4259,7 +4259,7 @@
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="41"/>
       <c r="B12" s="42">
-        <v>1.4</v>
+        <v>5</v>
       </c>
       <c r="C12" s="43">
         <v>2132.5</v>
@@ -4289,8 +4289,8 @@
         <v>1000000000</v>
       </c>
       <c r="L12" s="56">
-        <f>((R12+'Frequency Range Setting'!$B$2)*1000000)+$U$2</f>
-        <v>1736500000</v>
+        <f>((R12+'Frequency Range Setting'!$B$4)*1000000)+$U$2</f>
+        <v>1745500000</v>
       </c>
       <c r="M12" s="39">
         <v>150000</v>
@@ -4302,8 +4302,8 @@
         <v>1000000000</v>
       </c>
       <c r="P12" s="53">
-        <f>((R12-'Frequency Range Setting'!$B$2)*1000000)-$U$2</f>
-        <v>1728500000</v>
+        <f>((R12-'Frequency Range Setting'!$B$4)*1000000)-$U$2</f>
+        <v>1719500000</v>
       </c>
       <c r="Q12" s="39">
         <v>12750000000</v>
@@ -4316,7 +4316,7 @@
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="41"/>
       <c r="B13" s="42">
-        <v>1.4</v>
+        <v>5</v>
       </c>
       <c r="C13" s="43">
         <v>2132.5</v>
@@ -4325,7 +4325,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="41">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="F13" s="68">
         <v>-20</v>
@@ -4346,8 +4346,8 @@
         <v>1000000000</v>
       </c>
       <c r="L13" s="56">
-        <f>((R13+'Frequency Range Setting'!$B$2)*1000000)+$U$2</f>
-        <v>1736500000</v>
+        <f>((R13+'Frequency Range Setting'!$B$4)*1000000)+$U$2</f>
+        <v>1745500000</v>
       </c>
       <c r="M13" s="39">
         <v>150000</v>
@@ -4359,8 +4359,8 @@
         <v>1000000000</v>
       </c>
       <c r="P13" s="53">
-        <f>((R13-'Frequency Range Setting'!$B$2)*1000000)-$U$2</f>
-        <v>1728500000</v>
+        <f>((R13-'Frequency Range Setting'!$B$4)*1000000)-$U$2</f>
+        <v>1719500000</v>
       </c>
       <c r="Q13" s="39">
         <v>12750000000</v>
@@ -4373,13 +4373,13 @@
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="41"/>
       <c r="B14" s="42">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C14" s="43">
         <v>2132.5</v>
       </c>
       <c r="D14" s="41">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="E14" s="41">
         <v>0</v>
@@ -4403,8 +4403,8 @@
         <v>1000000000</v>
       </c>
       <c r="L14" s="56">
-        <f>((R14+'Frequency Range Setting'!$B$4)*1000000)+$U$2</f>
-        <v>1745500000</v>
+        <f>((R14+'Frequency Range Setting'!$B$7)*1000000)+$U$2</f>
+        <v>1768000000</v>
       </c>
       <c r="M14" s="39">
         <v>150000</v>
@@ -4416,8 +4416,8 @@
         <v>1000000000</v>
       </c>
       <c r="P14" s="53">
-        <f>((R14-'Frequency Range Setting'!$B$4)*1000000)-$U$2</f>
-        <v>1719500000</v>
+        <f>((R14-'Frequency Range Setting'!$B$7)*1000000)-$U$2</f>
+        <v>1697000000</v>
       </c>
       <c r="Q14" s="39">
         <v>12750000000</v>
@@ -4430,7 +4430,7 @@
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="41"/>
       <c r="B15" s="42">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C15" s="43">
         <v>2132.5</v>
@@ -4460,8 +4460,8 @@
         <v>1000000000</v>
       </c>
       <c r="L15" s="56">
-        <f>((R15+'Frequency Range Setting'!$B$4)*1000000)+$U$2</f>
-        <v>1745500000</v>
+        <f>((R15+'Frequency Range Setting'!$B$7)*1000000)+$U$2</f>
+        <v>1768000000</v>
       </c>
       <c r="M15" s="39">
         <v>150000</v>
@@ -4473,8 +4473,8 @@
         <v>1000000000</v>
       </c>
       <c r="P15" s="53">
-        <f>((R15-'Frequency Range Setting'!$B$4)*1000000)-$U$2</f>
-        <v>1719500000</v>
+        <f>((R15-'Frequency Range Setting'!$B$7)*1000000)-$U$2</f>
+        <v>1697000000</v>
       </c>
       <c r="Q15" s="39">
         <v>12750000000</v>
@@ -4487,7 +4487,7 @@
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="41"/>
       <c r="B16" s="42">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C16" s="43">
         <v>2132.5</v>
@@ -4496,7 +4496,7 @@
         <v>1</v>
       </c>
       <c r="E16" s="41">
-        <v>24</v>
+        <v>99</v>
       </c>
       <c r="F16" s="68">
         <v>-20</v>
@@ -4517,8 +4517,8 @@
         <v>1000000000</v>
       </c>
       <c r="L16" s="56">
-        <f>((R16+'Frequency Range Setting'!$B$4)*1000000)+$U$2</f>
-        <v>1745500000</v>
+        <f>((R16+'Frequency Range Setting'!$B$7)*1000000)+$U$2</f>
+        <v>1768000000</v>
       </c>
       <c r="M16" s="39">
         <v>150000</v>
@@ -4530,8 +4530,8 @@
         <v>1000000000</v>
       </c>
       <c r="P16" s="53">
-        <f>((R16-'Frequency Range Setting'!$B$4)*1000000)-$U$2</f>
-        <v>1719500000</v>
+        <f>((R16-'Frequency Range Setting'!$B$7)*1000000)-$U$2</f>
+        <v>1697000000</v>
       </c>
       <c r="Q16" s="39">
         <v>12750000000</v>
@@ -4542,24 +4542,24 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="41"/>
-      <c r="B17" s="42">
-        <v>20</v>
-      </c>
-      <c r="C17" s="43">
-        <v>2132.5</v>
-      </c>
-      <c r="D17" s="41">
-        <v>100</v>
-      </c>
-      <c r="E17" s="41">
+      <c r="A17" s="44"/>
+      <c r="B17" s="45">
+        <v>1.4</v>
+      </c>
+      <c r="C17" s="46">
+        <v>2154.3000000000002</v>
+      </c>
+      <c r="D17" s="44">
+        <v>6</v>
+      </c>
+      <c r="E17" s="44">
         <v>0</v>
       </c>
       <c r="F17" s="68">
         <v>-20</v>
       </c>
-      <c r="G17" s="42" t="s">
-        <v>8</v>
+      <c r="G17" s="45" t="s">
+        <v>9</v>
       </c>
       <c r="H17" s="39">
         <v>9000</v>
@@ -4574,8 +4574,8 @@
         <v>1000000000</v>
       </c>
       <c r="L17" s="56">
-        <f>((R17+'Frequency Range Setting'!$B$7)*1000000)+$U$2</f>
-        <v>1768000000</v>
+        <f>((R17+'Frequency Range Setting'!$B$2)*1000000)+$U$2</f>
+        <v>1758300000.0000002</v>
       </c>
       <c r="M17" s="39">
         <v>150000</v>
@@ -4587,36 +4587,36 @@
         <v>1000000000</v>
       </c>
       <c r="P17" s="53">
-        <f>((R17-'Frequency Range Setting'!$B$7)*1000000)-$U$2</f>
-        <v>1697000000</v>
+        <f>((R17-'Frequency Range Setting'!$B$2)*1000000)-$U$2</f>
+        <v>1750300000.0000002</v>
       </c>
       <c r="Q17" s="39">
         <v>12750000000</v>
       </c>
       <c r="R17" s="57">
         <f t="shared" si="0"/>
-        <v>1732.5</v>
+        <v>1754.3000000000002</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="41"/>
-      <c r="B18" s="42">
-        <v>20</v>
-      </c>
-      <c r="C18" s="43">
-        <v>2132.5</v>
-      </c>
-      <c r="D18" s="41">
-        <v>1</v>
-      </c>
-      <c r="E18" s="41">
+      <c r="A18" s="44"/>
+      <c r="B18" s="45">
+        <v>1.4</v>
+      </c>
+      <c r="C18" s="46">
+        <v>2154.3000000000002</v>
+      </c>
+      <c r="D18" s="44">
+        <v>1</v>
+      </c>
+      <c r="E18" s="44">
         <v>0</v>
       </c>
       <c r="F18" s="68">
         <v>-20</v>
       </c>
-      <c r="G18" s="42" t="s">
-        <v>8</v>
+      <c r="G18" s="45" t="s">
+        <v>9</v>
       </c>
       <c r="H18" s="39">
         <v>9000</v>
@@ -4631,8 +4631,8 @@
         <v>1000000000</v>
       </c>
       <c r="L18" s="56">
-        <f>((R18+'Frequency Range Setting'!$B$7)*1000000)+$U$2</f>
-        <v>1768000000</v>
+        <f>((R18+'Frequency Range Setting'!$B$2)*1000000)+$U$2</f>
+        <v>1758300000.0000002</v>
       </c>
       <c r="M18" s="39">
         <v>150000</v>
@@ -4644,36 +4644,36 @@
         <v>1000000000</v>
       </c>
       <c r="P18" s="53">
-        <f>((R18-'Frequency Range Setting'!$B$7)*1000000)-$U$2</f>
-        <v>1697000000</v>
+        <f>((R18-'Frequency Range Setting'!$B$2)*1000000)-$U$2</f>
+        <v>1750300000.0000002</v>
       </c>
       <c r="Q18" s="39">
         <v>12750000000</v>
       </c>
       <c r="R18" s="57">
         <f t="shared" si="0"/>
-        <v>1732.5</v>
+        <v>1754.3000000000002</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
-      <c r="B19" s="42">
-        <v>20</v>
-      </c>
-      <c r="C19" s="43">
-        <v>2132.5</v>
-      </c>
-      <c r="D19" s="41">
-        <v>1</v>
-      </c>
-      <c r="E19" s="41">
-        <v>99</v>
+      <c r="A19" s="44"/>
+      <c r="B19" s="45">
+        <v>1.4</v>
+      </c>
+      <c r="C19" s="46">
+        <v>2154.3000000000002</v>
+      </c>
+      <c r="D19" s="44">
+        <v>1</v>
+      </c>
+      <c r="E19" s="44">
+        <v>5</v>
       </c>
       <c r="F19" s="68">
         <v>-20</v>
       </c>
-      <c r="G19" s="42" t="s">
-        <v>8</v>
+      <c r="G19" s="45" t="s">
+        <v>9</v>
       </c>
       <c r="H19" s="39">
         <v>9000</v>
@@ -4688,8 +4688,8 @@
         <v>1000000000</v>
       </c>
       <c r="L19" s="56">
-        <f>((R19+'Frequency Range Setting'!$B$7)*1000000)+$U$2</f>
-        <v>1768000000</v>
+        <f>((R19+'Frequency Range Setting'!$B$2)*1000000)+$U$2</f>
+        <v>1758300000.0000002</v>
       </c>
       <c r="M19" s="39">
         <v>150000</v>
@@ -4701,27 +4701,27 @@
         <v>1000000000</v>
       </c>
       <c r="P19" s="53">
-        <f>((R19-'Frequency Range Setting'!$B$7)*1000000)-$U$2</f>
-        <v>1697000000</v>
+        <f>((R19-'Frequency Range Setting'!$B$2)*1000000)-$U$2</f>
+        <v>1750300000.0000002</v>
       </c>
       <c r="Q19" s="39">
         <v>12750000000</v>
       </c>
       <c r="R19" s="57">
         <f t="shared" si="0"/>
-        <v>1732.5</v>
+        <v>1754.3000000000002</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="44"/>
       <c r="B20" s="45">
-        <v>1.4</v>
+        <v>5</v>
       </c>
       <c r="C20" s="46">
-        <v>2154.3000000000002</v>
+        <v>2152.5</v>
       </c>
       <c r="D20" s="44">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E20" s="44">
         <v>0</v>
@@ -4745,8 +4745,8 @@
         <v>1000000000</v>
       </c>
       <c r="L20" s="56">
-        <f>((R20+'Frequency Range Setting'!$B$2)*1000000)+$U$2</f>
-        <v>1758300000.0000002</v>
+        <f>((R20+'Frequency Range Setting'!$B$4)*1000000)+$U$2</f>
+        <v>1765500000</v>
       </c>
       <c r="M20" s="39">
         <v>150000</v>
@@ -4758,24 +4758,24 @@
         <v>1000000000</v>
       </c>
       <c r="P20" s="53">
-        <f>((R20-'Frequency Range Setting'!$B$2)*1000000)-$U$2</f>
-        <v>1750300000.0000002</v>
+        <f>((R20-'Frequency Range Setting'!$B$4)*1000000)-$U$2</f>
+        <v>1739500000</v>
       </c>
       <c r="Q20" s="39">
         <v>12750000000</v>
       </c>
       <c r="R20" s="57">
         <f t="shared" si="0"/>
-        <v>1754.3000000000002</v>
+        <v>1752.5</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="44"/>
       <c r="B21" s="45">
-        <v>1.4</v>
+        <v>5</v>
       </c>
       <c r="C21" s="46">
-        <v>2154.3000000000002</v>
+        <v>2152.5</v>
       </c>
       <c r="D21" s="44">
         <v>1</v>
@@ -4802,8 +4802,8 @@
         <v>1000000000</v>
       </c>
       <c r="L21" s="56">
-        <f>((R21+'Frequency Range Setting'!$B$2)*1000000)+$U$2</f>
-        <v>1758300000.0000002</v>
+        <f>((R21+'Frequency Range Setting'!$B$4)*1000000)+$U$2</f>
+        <v>1765500000</v>
       </c>
       <c r="M21" s="39">
         <v>150000</v>
@@ -4815,36 +4815,36 @@
         <v>1000000000</v>
       </c>
       <c r="P21" s="53">
-        <f>((R21-'Frequency Range Setting'!$B$2)*1000000)-$U$2</f>
-        <v>1750300000.0000002</v>
+        <f>((R21-'Frequency Range Setting'!$B$4)*1000000)-$U$2</f>
+        <v>1739500000</v>
       </c>
       <c r="Q21" s="39">
         <v>12750000000</v>
       </c>
       <c r="R21" s="57">
         <f t="shared" si="0"/>
-        <v>1754.3000000000002</v>
+        <v>1752.5</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="44"/>
-      <c r="B22" s="45">
-        <v>1.4</v>
-      </c>
-      <c r="C22" s="46">
-        <v>2154.3000000000002</v>
-      </c>
-      <c r="D22" s="44">
-        <v>1</v>
-      </c>
-      <c r="E22" s="44">
-        <v>5</v>
+      <c r="A22" s="51"/>
+      <c r="B22" s="39">
+        <v>20</v>
+      </c>
+      <c r="C22" s="52">
+        <v>2120</v>
+      </c>
+      <c r="D22" s="51">
+        <v>100</v>
+      </c>
+      <c r="E22" s="51">
+        <v>0</v>
       </c>
       <c r="F22" s="68">
         <v>-20</v>
       </c>
-      <c r="G22" s="45" t="s">
-        <v>9</v>
+      <c r="G22" s="39" t="s">
+        <v>7</v>
       </c>
       <c r="H22" s="39">
         <v>9000</v>
@@ -4859,8 +4859,8 @@
         <v>1000000000</v>
       </c>
       <c r="L22" s="56">
-        <f>((R22+'Frequency Range Setting'!$B$2)*1000000)+$U$2</f>
-        <v>1758300000.0000002</v>
+        <f>((R22+'Frequency Range Setting'!$B$7)*1000000)+$U$2</f>
+        <v>1755500000</v>
       </c>
       <c r="M22" s="39">
         <v>150000</v>
@@ -4872,36 +4872,36 @@
         <v>1000000000</v>
       </c>
       <c r="P22" s="53">
-        <f>((R22-'Frequency Range Setting'!$B$2)*1000000)-$U$2</f>
-        <v>1750300000.0000002</v>
+        <f>((R22-'Frequency Range Setting'!$B$7)*1000000)-$U$2</f>
+        <v>1684500000</v>
       </c>
       <c r="Q22" s="39">
         <v>12750000000</v>
       </c>
       <c r="R22" s="57">
-        <f t="shared" si="0"/>
-        <v>1754.3000000000002</v>
+        <f>C22-400</f>
+        <v>1720</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
-      <c r="B23" s="45">
-        <v>5</v>
-      </c>
-      <c r="C23" s="46">
-        <v>2152.5</v>
-      </c>
-      <c r="D23" s="44">
-        <v>25</v>
-      </c>
-      <c r="E23" s="44">
+      <c r="A23" s="51"/>
+      <c r="B23" s="39">
+        <v>20</v>
+      </c>
+      <c r="C23" s="52">
+        <v>2120</v>
+      </c>
+      <c r="D23" s="51">
+        <v>1</v>
+      </c>
+      <c r="E23" s="51">
         <v>0</v>
       </c>
       <c r="F23" s="68">
         <v>-20</v>
       </c>
-      <c r="G23" s="45" t="s">
-        <v>9</v>
+      <c r="G23" s="39" t="s">
+        <v>7</v>
       </c>
       <c r="H23" s="39">
         <v>9000</v>
@@ -4916,8 +4916,8 @@
         <v>1000000000</v>
       </c>
       <c r="L23" s="56">
-        <f>((R23+'Frequency Range Setting'!$B$4)*1000000)+$U$2</f>
-        <v>1765500000</v>
+        <f>((R23+'Frequency Range Setting'!$B$7)*1000000)+$U$2</f>
+        <v>1755500000</v>
       </c>
       <c r="M23" s="39">
         <v>150000</v>
@@ -4929,36 +4929,36 @@
         <v>1000000000</v>
       </c>
       <c r="P23" s="53">
-        <f>((R23-'Frequency Range Setting'!$B$4)*1000000)-$U$2</f>
-        <v>1739500000</v>
+        <f>((R23-'Frequency Range Setting'!$B$7)*1000000)-$U$2</f>
+        <v>1684500000</v>
       </c>
       <c r="Q23" s="39">
         <v>12750000000</v>
       </c>
       <c r="R23" s="57">
-        <f t="shared" si="0"/>
-        <v>1752.5</v>
+        <f>C23-400</f>
+        <v>1720</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A24" s="44"/>
-      <c r="B24" s="45">
-        <v>5</v>
-      </c>
-      <c r="C24" s="46">
-        <v>2152.5</v>
-      </c>
-      <c r="D24" s="44">
-        <v>1</v>
-      </c>
-      <c r="E24" s="44">
-        <v>0</v>
+      <c r="A24" s="51"/>
+      <c r="B24" s="39">
+        <v>20</v>
+      </c>
+      <c r="C24" s="52">
+        <v>2120</v>
+      </c>
+      <c r="D24" s="51">
+        <v>1</v>
+      </c>
+      <c r="E24" s="51">
+        <v>99</v>
       </c>
       <c r="F24" s="68">
         <v>-20</v>
       </c>
-      <c r="G24" s="45" t="s">
-        <v>9</v>
+      <c r="G24" s="39" t="s">
+        <v>7</v>
       </c>
       <c r="H24" s="39">
         <v>9000</v>
@@ -4973,8 +4973,8 @@
         <v>1000000000</v>
       </c>
       <c r="L24" s="56">
-        <f>((R24+'Frequency Range Setting'!$B$4)*1000000)+$U$2</f>
-        <v>1765500000</v>
+        <f>((R24+'Frequency Range Setting'!$B$7)*1000000)+$U$2</f>
+        <v>1755500000</v>
       </c>
       <c r="M24" s="39">
         <v>150000</v>
@@ -4986,15 +4986,15 @@
         <v>1000000000</v>
       </c>
       <c r="P24" s="53">
-        <f>((R24-'Frequency Range Setting'!$B$4)*1000000)-$U$2</f>
-        <v>1739500000</v>
+        <f>((R24-'Frequency Range Setting'!$B$7)*1000000)-$U$2</f>
+        <v>1684500000</v>
       </c>
       <c r="Q24" s="39">
         <v>12750000000</v>
       </c>
       <c r="R24" s="57">
-        <f t="shared" si="0"/>
-        <v>1752.5</v>
+        <f>C24-400</f>
+        <v>1720</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
@@ -9381,7 +9381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F7206B6-36E5-4637-B4E1-0FEA65E91330}">
   <dimension ref="A1:U28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>

</xml_diff>